<commit_message>
Save minor modification in A1_Solution
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AE51BF-1575-4640-93F9-9302D434A207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31E4E88-AF6F-B346-842D-BE0283436B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="19200" windowHeight="19180" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="9" r:id="rId1"/>
@@ -349,7 +349,44 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - K6
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> - K7
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
           <t>unit_tests:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -4158,11 +4195,11 @@
       </c>
       <c r="C3" s="94">
         <f t="shared" ref="C3:C28" ca="1" si="0">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$3, $I$3)),0), 2)</f>
-        <v>63.41</v>
+        <v>50.46</v>
       </c>
       <c r="D3">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C5)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E3" s="33">
         <f>LN('Raw Data'!C5)</f>
@@ -4194,11 +4231,11 @@
       </c>
       <c r="C4" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>85.49</v>
+        <v>58.79</v>
       </c>
       <c r="D4">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C6)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="33">
         <f>LN('Raw Data'!C6)</f>
@@ -4219,11 +4256,11 @@
       </c>
       <c r="C5" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>66.819999999999993</v>
+        <v>99.1</v>
       </c>
       <c r="D5">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C7)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="33">
         <f>LN('Raw Data'!C7)</f>
@@ -4240,11 +4277,11 @@
       </c>
       <c r="C6" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>84.78</v>
+        <v>84.69</v>
       </c>
       <c r="D6">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C8)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E6" s="33">
         <f>LN('Raw Data'!C8)</f>
@@ -4273,11 +4310,11 @@
       </c>
       <c r="C7" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>74.599999999999994</v>
+        <v>71.739999999999995</v>
       </c>
       <c r="D7">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C9)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7" s="33">
         <f>LN('Raw Data'!C9)</f>
@@ -4307,11 +4344,11 @@
       </c>
       <c r="C8" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>34.72</v>
+        <v>67.23</v>
       </c>
       <c r="D8">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C10)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E8" s="33">
         <f>LN('Raw Data'!C10)</f>
@@ -4343,11 +4380,11 @@
       </c>
       <c r="C9" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>66.38</v>
+        <v>61.01</v>
       </c>
       <c r="D9">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C11)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E9" s="33">
         <f>LN('Raw Data'!C11)</f>
@@ -4368,7 +4405,7 @@
       </c>
       <c r="C10" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>80.12</v>
+        <v>30.66</v>
       </c>
       <c r="D10">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C12)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4399,11 +4436,11 @@
       </c>
       <c r="C11" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>32.25</v>
+        <v>30.68</v>
       </c>
       <c r="D11">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C13)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="33">
         <f>LN('Raw Data'!C13)</f>
@@ -4431,11 +4468,11 @@
       </c>
       <c r="C12" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>79.819999999999993</v>
+        <v>21.81</v>
       </c>
       <c r="D12">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C14)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E12" s="33">
         <f>LN('Raw Data'!C14)</f>
@@ -4459,11 +4496,11 @@
       </c>
       <c r="C13" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>69.510000000000005</v>
+        <v>65.819999999999993</v>
       </c>
       <c r="D13">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C15)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E13" s="33">
         <f>LN('Raw Data'!C15)</f>
@@ -4487,11 +4524,11 @@
       </c>
       <c r="C14" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>62.32</v>
+        <v>39.29</v>
       </c>
       <c r="D14">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C16)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E14" s="33">
         <f>LN('Raw Data'!C16)</f>
@@ -4508,11 +4545,11 @@
       </c>
       <c r="C15" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>24.11</v>
+        <v>86.71</v>
       </c>
       <c r="D15">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C17)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="33">
         <f>LN('Raw Data'!C17)</f>
@@ -4529,7 +4566,7 @@
       </c>
       <c r="C16" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>68.41</v>
+        <v>68.540000000000006</v>
       </c>
       <c r="D16">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C18)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4550,11 +4587,11 @@
       </c>
       <c r="C17" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>54.67</v>
+        <v>97.52</v>
       </c>
       <c r="D17">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C19)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E17" s="33">
         <f>LN('Raw Data'!C19)</f>
@@ -4571,11 +4608,11 @@
       </c>
       <c r="C18" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>45.65</v>
+        <v>90.9</v>
       </c>
       <c r="D18">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C20)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E18" s="33">
         <f>LN('Raw Data'!C20)</f>
@@ -4592,11 +4629,11 @@
       </c>
       <c r="C19" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>80.290000000000006</v>
+        <v>78.52</v>
       </c>
       <c r="D19">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C21)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="33">
         <f>LN('Raw Data'!C21)</f>
@@ -4613,11 +4650,11 @@
       </c>
       <c r="C20" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>50.85</v>
+        <v>65.12</v>
       </c>
       <c r="D20">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C22)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E20" s="33">
         <f>LN('Raw Data'!C22)</f>
@@ -4634,11 +4671,11 @@
       </c>
       <c r="C21" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>66.91</v>
+        <v>68.81</v>
       </c>
       <c r="D21">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C23)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E21" s="33">
         <f>LN('Raw Data'!C23)</f>
@@ -4655,11 +4692,11 @@
       </c>
       <c r="C22" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>58.79</v>
+        <v>74.89</v>
       </c>
       <c r="D22">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C24)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E22" s="33">
         <f>LN('Raw Data'!C24)</f>
@@ -4676,11 +4713,11 @@
       </c>
       <c r="C23" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>63.39</v>
+        <v>72.680000000000007</v>
       </c>
       <c r="D23">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C25)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E23" s="33">
         <f>LN('Raw Data'!C25)</f>
@@ -4697,11 +4734,11 @@
       </c>
       <c r="C24" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>57.18</v>
+        <v>29.31</v>
       </c>
       <c r="D24">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C26)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E24" s="33">
         <f>LN('Raw Data'!C26)</f>
@@ -4718,11 +4755,11 @@
       </c>
       <c r="C25" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>51.61</v>
+        <v>27.27</v>
       </c>
       <c r="D25">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C27)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E25" s="33">
         <f>LN('Raw Data'!C27)</f>
@@ -4739,11 +4776,11 @@
       </c>
       <c r="C26" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>61.4</v>
+        <v>64.819999999999993</v>
       </c>
       <c r="D26">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C28)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E26" s="33">
         <f>LN('Raw Data'!C28)</f>
@@ -4760,11 +4797,11 @@
       </c>
       <c r="C27" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>72.37</v>
+        <v>52.01</v>
       </c>
       <c r="D27">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C29)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E27" s="33">
         <f>LN('Raw Data'!C29)</f>
@@ -4781,11 +4818,11 @@
       </c>
       <c r="C28" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>6.82</v>
+        <v>50.08</v>
       </c>
       <c r="D28">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C30)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E28" s="33">
         <f>LN('Raw Data'!C30)</f>
@@ -4802,7 +4839,7 @@
       </c>
       <c r="C29" s="94">
         <f t="shared" ref="C29:C54" ca="1" si="2">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$8, $I$8)),0), 2)</f>
-        <v>31.22</v>
+        <v>65.040000000000006</v>
       </c>
       <c r="D29">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C31)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4823,7 +4860,7 @@
       </c>
       <c r="C30" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>96.88</v>
+        <v>45.01</v>
       </c>
       <c r="D30">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C32)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4844,11 +4881,11 @@
       </c>
       <c r="C31" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>80.459999999999994</v>
+        <v>53.03</v>
       </c>
       <c r="D31">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C33)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E31" s="33">
         <f>LN('Raw Data'!C33)</f>
@@ -4865,11 +4902,11 @@
       </c>
       <c r="C32" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>58.85</v>
+        <v>81.680000000000007</v>
       </c>
       <c r="D32">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C34)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E32" s="33">
         <f>LN('Raw Data'!C34)</f>
@@ -4886,11 +4923,11 @@
       </c>
       <c r="C33" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>62.54</v>
+        <v>77.53</v>
       </c>
       <c r="D33">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C35)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E33" s="33">
         <f>LN('Raw Data'!C35)</f>
@@ -4907,7 +4944,7 @@
       </c>
       <c r="C34" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>11.15</v>
+        <v>54.77</v>
       </c>
       <c r="D34">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C36)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4928,11 +4965,11 @@
       </c>
       <c r="C35" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>50.13</v>
+        <v>91.16</v>
       </c>
       <c r="D35">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C37)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E35" s="33">
         <f>LN('Raw Data'!C37)</f>
@@ -4949,11 +4986,11 @@
       </c>
       <c r="C36" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>72.56</v>
+        <v>30.21</v>
       </c>
       <c r="D36">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C38)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E36" s="33">
         <f>LN('Raw Data'!C38)</f>
@@ -4970,11 +5007,11 @@
       </c>
       <c r="C37" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>73.239999999999995</v>
+        <v>46.77</v>
       </c>
       <c r="D37">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C39)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E37" s="33">
         <f>LN('Raw Data'!C39)</f>
@@ -4991,11 +5028,11 @@
       </c>
       <c r="C38" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>30.3</v>
+        <v>43.33</v>
       </c>
       <c r="D38">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C40)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E38" s="33">
         <f>LN('Raw Data'!C40)</f>
@@ -5012,11 +5049,11 @@
       </c>
       <c r="C39" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>55.54</v>
+        <v>73.94</v>
       </c>
       <c r="D39">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C41)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E39" s="33">
         <f>LN('Raw Data'!C41)</f>
@@ -5033,11 +5070,11 @@
       </c>
       <c r="C40" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>71.92</v>
+        <v>90.82</v>
       </c>
       <c r="D40">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C42)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E40" s="33">
         <f>LN('Raw Data'!C42)</f>
@@ -5054,11 +5091,11 @@
       </c>
       <c r="C41" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>47.87</v>
+        <v>33.35</v>
       </c>
       <c r="D41">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C43)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E41" s="33">
         <f>LN('Raw Data'!C43)</f>
@@ -5075,11 +5112,11 @@
       </c>
       <c r="C42" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>84.66</v>
+        <v>37.869999999999997</v>
       </c>
       <c r="D42">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C44)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E42" s="33">
         <f>LN('Raw Data'!C44)</f>
@@ -5096,11 +5133,11 @@
       </c>
       <c r="C43" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>52.76</v>
+        <v>77.819999999999993</v>
       </c>
       <c r="D43">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C45)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E43" s="33">
         <f>LN('Raw Data'!C45)</f>
@@ -5117,11 +5154,11 @@
       </c>
       <c r="C44" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>38.840000000000003</v>
+        <v>62.54</v>
       </c>
       <c r="D44">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C46)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E44" s="33">
         <f>LN('Raw Data'!C46)</f>
@@ -5138,11 +5175,11 @@
       </c>
       <c r="C45" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>12.41</v>
+        <v>29.48</v>
       </c>
       <c r="D45">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C47)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E45" s="33">
         <f>LN('Raw Data'!C47)</f>
@@ -5159,11 +5196,11 @@
       </c>
       <c r="C46" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>25.48</v>
       </c>
       <c r="D46">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C48)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E46" s="33">
         <f>LN('Raw Data'!C48)</f>
@@ -5180,11 +5217,11 @@
       </c>
       <c r="C47" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>56.66</v>
+        <v>48.86</v>
       </c>
       <c r="D47">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C49)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E47" s="33">
         <f>LN('Raw Data'!C49)</f>
@@ -5201,11 +5238,11 @@
       </c>
       <c r="C48" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>24.79</v>
+        <v>41.96</v>
       </c>
       <c r="D48">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C50)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E48" s="33">
         <f>LN('Raw Data'!C50)</f>
@@ -5222,11 +5259,11 @@
       </c>
       <c r="C49" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>52.82</v>
+        <v>49.06</v>
       </c>
       <c r="D49">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C51)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E49" s="33">
         <f>LN('Raw Data'!C51)</f>
@@ -5243,11 +5280,11 @@
       </c>
       <c r="C50" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>27.7</v>
+        <v>72.11</v>
       </c>
       <c r="D50">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C52)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E50" s="33">
         <f>LN('Raw Data'!C52)</f>
@@ -5264,11 +5301,11 @@
       </c>
       <c r="C51" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>64.069999999999993</v>
+        <v>58.2</v>
       </c>
       <c r="D51">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C53)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E51" s="33">
         <f>LN('Raw Data'!C53)</f>
@@ -5285,11 +5322,11 @@
       </c>
       <c r="C52" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>15.62</v>
+        <v>100</v>
       </c>
       <c r="D52">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C54)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E52" s="33">
         <f>LN('Raw Data'!C54)</f>
@@ -5306,11 +5343,11 @@
       </c>
       <c r="C53" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>1.99</v>
+        <v>94.56</v>
       </c>
       <c r="D53">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C55)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E53" s="33">
         <f>LN('Raw Data'!C55)</f>
@@ -5327,11 +5364,11 @@
       </c>
       <c r="C54" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>55.15</v>
+        <v>48.4</v>
       </c>
       <c r="D54">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C56)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E54" s="33">
         <f>LN('Raw Data'!C56)</f>
@@ -5371,7 +5408,7 @@
       </c>
       <c r="B59" s="33">
         <f ca="1">AVERAGEA($C$3:$C$28)</f>
-        <v>60.102692307692323</v>
+        <v>61.86384615384614</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -5380,7 +5417,7 @@
       </c>
       <c r="B60" s="33">
         <f ca="1">AVERAGEA($C$29:$C$54)</f>
-        <v>51.158846153846149</v>
+        <v>58.960769230769223</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -5389,7 +5426,7 @@
       </c>
       <c r="B61" s="33">
         <f ca="1">STDEVA($C$3:$C$28)</f>
-        <v>19.067066592990578</v>
+        <v>22.045653009502519</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13">
@@ -5398,7 +5435,7 @@
       </c>
       <c r="B62" s="33">
         <f ca="1">STDEVA($C$29:$C$54)</f>
-        <v>26.293838719657948</v>
+        <v>21.749410092795983</v>
       </c>
     </row>
   </sheetData>
@@ -7911,8 +7948,8 @@
   </sheetPr>
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="268" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add alternative cells in A1_Solution
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31E4E88-AF6F-B346-842D-BE0283436B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB4F613-709B-4949-88D8-D3A8C653FCA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="19200" windowHeight="19180" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="15740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="9" r:id="rId1"/>
@@ -26,6 +26,17 @@
     <sheet name="Random Data" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -359,7 +370,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> - K6
+          <t xml:space="preserve"> - P5
 </t>
         </r>
         <r>
@@ -368,7 +379,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> - K7
+          <t xml:space="preserve"> - Q5
 </t>
         </r>
         <r>
@@ -377,7 +388,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>unit_tests:</t>
+          <t xml:space="preserve"> - R5</t>
         </r>
         <r>
           <rPr>
@@ -386,6 +397,15 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">unit_tests:
 </t>
         </r>
       </text>
@@ -420,6 +440,75 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>alt_cells:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> - P5</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> - Q5</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> - R5</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -1618,7 +1707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1808,36 +1897,27 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1852,15 +1932,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1870,6 +1953,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3032,20 +3122,20 @@
     </row>
     <row r="2" spans="1:10" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="100" t="s">
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="I2" s="126" t="s">
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="I2" s="127" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:10" ht="13">
       <c r="A3" s="5"/>
@@ -3067,8 +3157,8 @@
       <c r="G3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="127"/>
-      <c r="J3" s="112"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="109"/>
     </row>
     <row r="4" spans="1:10" ht="13">
       <c r="B4" s="55">
@@ -3095,8 +3185,8 @@
         <f t="shared" ref="G4:G29" si="1">LN(F4)</f>
         <v>4.5860892981752999</v>
       </c>
-      <c r="I4" s="113"/>
-      <c r="J4" s="114"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="111"/>
     </row>
     <row r="5" spans="1:10" ht="13">
       <c r="B5" s="55">
@@ -3123,8 +3213,8 @@
         <f t="shared" si="1"/>
         <v>4.1437694455496237</v>
       </c>
-      <c r="I5" s="113"/>
-      <c r="J5" s="114"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="111"/>
     </row>
     <row r="6" spans="1:10" ht="13">
       <c r="B6" s="55">
@@ -3151,8 +3241,8 @@
         <f t="shared" si="1"/>
         <v>4.1436108035250188</v>
       </c>
-      <c r="I6" s="113"/>
-      <c r="J6" s="114"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="111"/>
     </row>
     <row r="7" spans="1:10" ht="13">
       <c r="B7" s="55">
@@ -3179,8 +3269,8 @@
         <f t="shared" si="1"/>
         <v>4.438643235092778</v>
       </c>
-      <c r="I7" s="113"/>
-      <c r="J7" s="114"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="111"/>
     </row>
     <row r="8" spans="1:10" ht="13">
       <c r="B8" s="55">
@@ -3207,8 +3297,8 @@
         <f t="shared" si="1"/>
         <v>3.942358205224219</v>
       </c>
-      <c r="I8" s="113"/>
-      <c r="J8" s="114"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="111"/>
     </row>
     <row r="9" spans="1:10" ht="13">
       <c r="B9" s="55">
@@ -3235,8 +3325,8 @@
         <f t="shared" si="1"/>
         <v>3.8486571298063263</v>
       </c>
-      <c r="I9" s="113"/>
-      <c r="J9" s="114"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="111"/>
     </row>
     <row r="10" spans="1:10" ht="13">
       <c r="B10" s="55">
@@ -3263,8 +3353,8 @@
         <f t="shared" si="1"/>
         <v>3.9425522104629689</v>
       </c>
-      <c r="I10" s="113"/>
-      <c r="J10" s="114"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="111"/>
     </row>
     <row r="11" spans="1:10" ht="13">
       <c r="B11" s="55">
@@ -3291,8 +3381,8 @@
         <f t="shared" si="1"/>
         <v>3.9502817175452365</v>
       </c>
-      <c r="I11" s="113"/>
-      <c r="J11" s="114"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="111"/>
     </row>
     <row r="12" spans="1:10" ht="13">
       <c r="B12" s="55">
@@ -3319,8 +3409,8 @@
         <f t="shared" si="1"/>
         <v>4.1052845022604352</v>
       </c>
-      <c r="I12" s="113"/>
-      <c r="J12" s="114"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="111"/>
     </row>
     <row r="13" spans="1:10" ht="13">
       <c r="B13" s="55">
@@ -3347,8 +3437,8 @@
         <f t="shared" si="1"/>
         <v>3.9932342608529692</v>
       </c>
-      <c r="I13" s="113"/>
-      <c r="J13" s="114"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="111"/>
     </row>
     <row r="14" spans="1:10" ht="13">
       <c r="B14" s="55">
@@ -3375,8 +3465,8 @@
         <f t="shared" si="1"/>
         <v>4.3330989610504584</v>
       </c>
-      <c r="I14" s="113"/>
-      <c r="J14" s="114"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="111"/>
     </row>
     <row r="15" spans="1:10" ht="13">
       <c r="B15" s="55">
@@ -3403,8 +3493,8 @@
         <f t="shared" si="1"/>
         <v>4.3899948043230586</v>
       </c>
-      <c r="I15" s="113"/>
-      <c r="J15" s="114"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="111"/>
     </row>
     <row r="16" spans="1:10" ht="13">
       <c r="B16" s="55">
@@ -3431,8 +3521,8 @@
         <f t="shared" si="1"/>
         <v>4.5332444464165027</v>
       </c>
-      <c r="I16" s="113"/>
-      <c r="J16" s="114"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="111"/>
     </row>
     <row r="17" spans="1:12" ht="13">
       <c r="B17" s="55">
@@ -3459,8 +3549,8 @@
         <f t="shared" si="1"/>
         <v>2.0386195471595809</v>
       </c>
-      <c r="I17" s="113"/>
-      <c r="J17" s="114"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="111"/>
     </row>
     <row r="18" spans="1:12" ht="13">
       <c r="B18" s="55">
@@ -3487,8 +3577,8 @@
         <f t="shared" si="1"/>
         <v>3.2872818575322613</v>
       </c>
-      <c r="I18" s="113"/>
-      <c r="J18" s="114"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="111"/>
     </row>
     <row r="19" spans="1:12" ht="13">
       <c r="B19" s="55">
@@ -3515,8 +3605,8 @@
         <f t="shared" si="1"/>
         <v>4.2756934238792645</v>
       </c>
-      <c r="I19" s="113"/>
-      <c r="J19" s="114"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="111"/>
     </row>
     <row r="20" spans="1:12" ht="13">
       <c r="B20" s="55">
@@ -3543,8 +3633,8 @@
         <f t="shared" si="1"/>
         <v>3.7972853279577228</v>
       </c>
-      <c r="I20" s="113"/>
-      <c r="J20" s="114"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="111"/>
     </row>
     <row r="21" spans="1:12" ht="13">
       <c r="B21" s="55">
@@ -3571,8 +3661,8 @@
         <f t="shared" si="1"/>
         <v>3.9442965659784419</v>
       </c>
-      <c r="I21" s="113"/>
-      <c r="J21" s="114"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="111"/>
     </row>
     <row r="22" spans="1:12" ht="13">
       <c r="B22" s="55">
@@ -3599,8 +3689,8 @@
         <f t="shared" si="1"/>
         <v>4.3384665199215018</v>
       </c>
-      <c r="I22" s="115"/>
-      <c r="J22" s="117"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="114"/>
     </row>
     <row r="23" spans="1:12" ht="13">
       <c r="B23" s="55">
@@ -3784,23 +3874,23 @@
         <v>4.0055133485154846</v>
       </c>
       <c r="H29" s="4"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="99"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="101"/>
     </row>
     <row r="30" spans="1:12" ht="13">
       <c r="H30" s="4"/>
-      <c r="I30" s="105"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="105"/>
-      <c r="L30" s="99"/>
+      <c r="I30" s="100"/>
+      <c r="J30" s="101"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="101"/>
     </row>
     <row r="31" spans="1:12" ht="13">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="99"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
@@ -3816,10 +3906,10 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A32" s="101" t="s">
+      <c r="A32" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="99"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="2">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -3843,13 +3933,13 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="99"/>
+      <c r="L32" s="101"/>
     </row>
     <row r="33" spans="1:12" ht="13">
-      <c r="A33" s="101" t="s">
+      <c r="A33" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="99"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="32">
         <f t="shared" ref="C33:D33" si="4">STDEVA(C$4:C$11, C$13:C$29)</f>
         <v>18.592928377925453</v>
@@ -3873,13 +3963,13 @@
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="99"/>
+      <c r="L33" s="101"/>
     </row>
     <row r="34" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A34" s="101" t="s">
+      <c r="A34" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="99"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="6">SKEW(C$4:C$11, C$13:C$29)</f>
         <v>0.24893711104029126</v>
@@ -3901,13 +3991,13 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="99"/>
+      <c r="L34" s="101"/>
     </row>
     <row r="35" spans="1:12" ht="13">
-      <c r="A35" s="101" t="s">
+      <c r="A35" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="99"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="8">MEDIAN(C$4:C$11, C$13:C$29)</f>
         <v>57.68</v>
@@ -3931,13 +4021,13 @@
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="99"/>
+      <c r="L35" s="101"/>
     </row>
     <row r="36" spans="1:12" ht="13">
-      <c r="A36" s="101" t="s">
+      <c r="A36" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="99"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="10">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -3962,13 +4052,13 @@
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="99"/>
+      <c r="L36" s="101"/>
     </row>
     <row r="37" spans="1:12" ht="13">
-      <c r="A37" s="101" t="s">
+      <c r="A37" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="99"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="12">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -3990,7 +4080,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="99"/>
+      <c r="L37" s="101"/>
     </row>
     <row r="38" spans="1:12" ht="13">
       <c r="A38" s="15"/>
@@ -4003,7 +4093,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="99"/>
+      <c r="L38" s="101"/>
     </row>
     <row r="39" spans="1:12" ht="13">
       <c r="A39" s="15"/>
@@ -4021,13 +4111,13 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="99"/>
+      <c r="L39" s="101"/>
     </row>
     <row r="40" spans="1:12" ht="15">
-      <c r="A40" s="101" t="s">
+      <c r="A40" s="102" t="s">
         <v>138</v>
       </c>
-      <c r="B40" s="99"/>
+      <c r="B40" s="101"/>
       <c r="C40" s="51">
         <f>SQRT((C33^2*(C31-1)+F33^2*(F31-1))/(C31+F31-2))</f>
         <v>20.89619836575601</v>
@@ -4043,13 +4133,13 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="99"/>
+      <c r="L40" s="101"/>
     </row>
     <row r="41" spans="1:12" ht="15">
-      <c r="A41" s="101" t="s">
+      <c r="A41" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="99"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="32">
         <f t="shared" ref="C41:D41" si="14">ABS(C32-F32)</f>
         <v>1</v>
@@ -4065,10 +4155,10 @@
       <c r="I41" s="92"/>
     </row>
     <row r="42" spans="1:12" ht="13">
-      <c r="A42" s="101" t="s">
+      <c r="A42" s="102" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="99"/>
+      <c r="B42" s="101"/>
       <c r="C42" s="32">
         <f t="shared" ref="C42:D42" si="15">SQRT(C33^2/$C31 + F33^2/$F31)</f>
         <v>5.7955626669230851</v>
@@ -4098,6 +4188,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J22"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="L32:L40"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
@@ -4106,16 +4206,6 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="L32:L40"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J22"/>
-    <mergeCell ref="I29:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4186,7 +4276,7 @@
         <v>0.16000000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4195,11 +4285,11 @@
       </c>
       <c r="C3" s="94">
         <f t="shared" ref="C3:C28" ca="1" si="0">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$3, $I$3)),0), 2)</f>
-        <v>50.46</v>
+        <v>55.03</v>
       </c>
       <c r="D3">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C5)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E3" s="33">
         <f>LN('Raw Data'!C5)</f>
@@ -4221,7 +4311,7 @@
         <v>606.97340451085847</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" s="5">
         <f t="shared" ref="A4:A54" si="1">A3+1</f>
         <v>2</v>
@@ -4231,11 +4321,11 @@
       </c>
       <c r="C4" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>58.79</v>
+        <v>7.29</v>
       </c>
       <c r="D4">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C6)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="33">
         <f>LN('Raw Data'!C6)</f>
@@ -4246,7 +4336,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -4256,18 +4346,18 @@
       </c>
       <c r="C5" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>99.1</v>
+        <v>38.53</v>
       </c>
       <c r="D5">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C7)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E5" s="33">
         <f>LN('Raw Data'!C7)</f>
         <v>4.5709927341865049</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4277,11 +4367,11 @@
       </c>
       <c r="C6" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>84.69</v>
+        <v>32.21</v>
       </c>
       <c r="D6">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C8)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E6" s="33">
         <f>LN('Raw Data'!C8)</f>
@@ -4300,7 +4390,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -4310,7 +4400,7 @@
       </c>
       <c r="C7" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>71.739999999999995</v>
+        <v>67.91</v>
       </c>
       <c r="D7">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C9)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4334,7 +4424,7 @@
         <v>0.148225</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4344,11 +4434,11 @@
       </c>
       <c r="C8" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>67.23</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C10)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="33">
         <f>LN('Raw Data'!C10)</f>
@@ -4370,7 +4460,7 @@
         <v>610.46983794715493</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="5">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4380,11 +4470,11 @@
       </c>
       <c r="C9" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>61.01</v>
+        <v>67.84</v>
       </c>
       <c r="D9">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C11)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E9" s="33">
         <f>LN('Raw Data'!C11)</f>
@@ -4395,7 +4485,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -4405,11 +4495,11 @@
       </c>
       <c r="C10" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>30.66</v>
+        <v>35.92</v>
       </c>
       <c r="D10">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C12)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E10" s="33">
         <f>LN('Raw Data'!C12)</f>
@@ -4426,7 +4516,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4436,11 +4526,11 @@
       </c>
       <c r="C11" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>30.68</v>
+        <v>45.67</v>
       </c>
       <c r="D11">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C13)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E11" s="33">
         <f>LN('Raw Data'!C13)</f>
@@ -4458,7 +4548,7 @@
       <c r="J11" s="21"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4468,7 +4558,7 @@
       </c>
       <c r="C12" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>21.81</v>
+        <v>68.349999999999994</v>
       </c>
       <c r="D12">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C14)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4486,7 +4576,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -4496,11 +4586,11 @@
       </c>
       <c r="C13" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>65.819999999999993</v>
+        <v>65.650000000000006</v>
       </c>
       <c r="D13">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C15)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E13" s="33">
         <f>LN('Raw Data'!C15)</f>
@@ -4514,7 +4604,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -4524,18 +4614,18 @@
       </c>
       <c r="C14" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>39.29</v>
+        <v>63.33</v>
       </c>
       <c r="D14">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C16)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E14" s="33">
         <f>LN('Raw Data'!C16)</f>
         <v>4.1999050578825932</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -4545,18 +4635,18 @@
       </c>
       <c r="C15" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>86.71</v>
+        <v>67.94</v>
       </c>
       <c r="D15">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C17)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E15" s="33">
         <f>LN('Raw Data'!C17)</f>
         <v>3.9304521408965134</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4566,18 +4656,18 @@
       </c>
       <c r="C16" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>68.540000000000006</v>
+        <v>80.05</v>
       </c>
       <c r="D16">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C18)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E16" s="33">
         <f>LN('Raw Data'!C18)</f>
         <v>3.9485477801105184</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -4587,18 +4677,18 @@
       </c>
       <c r="C17" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>97.52</v>
+        <v>56.11</v>
       </c>
       <c r="D17">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C19)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17" s="33">
         <f>LN('Raw Data'!C19)</f>
         <v>3.7357630400127868</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -4608,18 +4698,18 @@
       </c>
       <c r="C18" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>90.9</v>
+        <v>86.35</v>
       </c>
       <c r="D18">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C20)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E18" s="33">
         <f>LN('Raw Data'!C20)</f>
         <v>2.6979998652487085</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -4629,18 +4719,18 @@
       </c>
       <c r="C19" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>78.52</v>
+        <v>66.05</v>
       </c>
       <c r="D19">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C21)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E19" s="33">
         <f>LN('Raw Data'!C21)</f>
         <v>4.1277793383083381</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="5">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -4650,18 +4740,18 @@
       </c>
       <c r="C20" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>65.12</v>
+        <v>64.069999999999993</v>
       </c>
       <c r="D20">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C22)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" s="33">
         <f>LN('Raw Data'!C22)</f>
         <v>3.8940626800511531</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -4671,18 +4761,18 @@
       </c>
       <c r="C21" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>68.81</v>
+        <v>61.25</v>
       </c>
       <c r="D21">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C23)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E21" s="33">
         <f>LN('Raw Data'!C23)</f>
         <v>4.110217911378391</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="15">
       <c r="A22" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -4692,18 +4782,18 @@
       </c>
       <c r="C22" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>74.89</v>
+        <v>72.12</v>
       </c>
       <c r="D22">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C24)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E22" s="33">
         <f>LN('Raw Data'!C24)</f>
         <v>4.2158244597598102</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="15">
       <c r="A23" s="5">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -4713,18 +4803,18 @@
       </c>
       <c r="C23" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>72.680000000000007</v>
+        <v>87.71</v>
       </c>
       <c r="D23">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C25)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="33">
         <f>LN('Raw Data'!C25)</f>
         <v>4.0549104929766937</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="15">
       <c r="A24" s="5">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -4734,18 +4824,18 @@
       </c>
       <c r="C24" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>29.31</v>
+        <v>57.22</v>
       </c>
       <c r="D24">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C26)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E24" s="33">
         <f>LN('Raw Data'!C26)</f>
         <v>4.2413267525707461</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="15">
       <c r="A25" s="5">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -4755,18 +4845,18 @@
       </c>
       <c r="C25" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>27.27</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="D25">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C27)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E25" s="33">
         <f>LN('Raw Data'!C27)</f>
         <v>4.0455043968026274</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="15">
       <c r="A26" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -4776,18 +4866,18 @@
       </c>
       <c r="C26" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>64.819999999999993</v>
+        <v>54.44</v>
       </c>
       <c r="D26">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C28)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E26" s="33">
         <f>LN('Raw Data'!C28)</f>
         <v>3.7106409458954492</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="15">
       <c r="A27" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -4797,18 +4887,18 @@
       </c>
       <c r="C27" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>52.01</v>
+        <v>18.57</v>
       </c>
       <c r="D27">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C29)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E27" s="33">
         <f>LN('Raw Data'!C29)</f>
         <v>3.9961803134348695</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="15">
       <c r="A28" s="5">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -4818,18 +4908,18 @@
       </c>
       <c r="C28" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>50.08</v>
+        <v>34.81</v>
       </c>
       <c r="D28">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C30)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E28" s="33">
         <f>LN('Raw Data'!C30)</f>
         <v>4.1108738641733114</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="15">
       <c r="A29" s="5">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -4839,18 +4929,18 @@
       </c>
       <c r="C29" s="94">
         <f t="shared" ref="C29:C54" ca="1" si="2">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$8, $I$8)),0), 2)</f>
-        <v>65.040000000000006</v>
+        <v>96.19</v>
       </c>
       <c r="D29">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C31)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E29" s="33">
         <f>LN('Raw Data'!C31)</f>
         <v>4.5860892981752999</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="15">
       <c r="A30" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -4860,18 +4950,18 @@
       </c>
       <c r="C30" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>45.01</v>
+        <v>42.38</v>
       </c>
       <c r="D30">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C32)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E30" s="33">
         <f>LN('Raw Data'!C32)</f>
         <v>4.1437694455496237</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" ht="15">
       <c r="A31" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -4881,18 +4971,18 @@
       </c>
       <c r="C31" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>53.03</v>
+        <v>72.56</v>
       </c>
       <c r="D31">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C33)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E31" s="33">
         <f>LN('Raw Data'!C33)</f>
         <v>4.1436108035250188</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="15">
       <c r="A32" s="5">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -4902,18 +4992,18 @@
       </c>
       <c r="C32" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>81.680000000000007</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="D32">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C34)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" s="33">
         <f>LN('Raw Data'!C34)</f>
         <v>4.438643235092778</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="15">
       <c r="A33" s="5">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -4923,18 +5013,18 @@
       </c>
       <c r="C33" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>77.53</v>
+        <v>60.98</v>
       </c>
       <c r="D33">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C35)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E33" s="33">
         <f>LN('Raw Data'!C35)</f>
         <v>3.942358205224219</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" ht="15">
       <c r="A34" s="5">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -4944,18 +5034,18 @@
       </c>
       <c r="C34" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>54.77</v>
+        <v>100</v>
       </c>
       <c r="D34">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C36)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E34" s="33">
         <f>LN('Raw Data'!C36)</f>
         <v>3.8486571298063263</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" ht="15">
       <c r="A35" s="5">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -4965,18 +5055,18 @@
       </c>
       <c r="C35" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>91.16</v>
+        <v>54.47</v>
       </c>
       <c r="D35">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C37)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E35" s="33">
         <f>LN('Raw Data'!C37)</f>
         <v>3.9425522104629689</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" ht="15">
       <c r="A36" s="5">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -4986,18 +5076,18 @@
       </c>
       <c r="C36" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>30.21</v>
+        <v>54.01</v>
       </c>
       <c r="D36">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C38)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E36" s="33">
         <f>LN('Raw Data'!C38)</f>
         <v>3.9502817175452365</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" ht="15">
       <c r="A37" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -5007,18 +5097,18 @@
       </c>
       <c r="C37" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>46.77</v>
+        <v>54.55</v>
       </c>
       <c r="D37">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C39)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E37" s="33">
         <f>LN('Raw Data'!C39)</f>
         <v>4.1052845022604352</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="15">
       <c r="A38" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -5028,18 +5118,18 @@
       </c>
       <c r="C38" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>43.33</v>
+        <v>99.88</v>
       </c>
       <c r="D38">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C40)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E38" s="33">
         <f>LN('Raw Data'!C40)</f>
         <v>3.9932342608529692</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" ht="15">
       <c r="A39" s="5">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -5049,18 +5139,18 @@
       </c>
       <c r="C39" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>73.94</v>
+        <v>74.92</v>
       </c>
       <c r="D39">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C41)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E39" s="33">
         <f>LN('Raw Data'!C41)</f>
         <v>4.3330989610504584</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" ht="15">
       <c r="A40" s="5">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -5070,18 +5160,18 @@
       </c>
       <c r="C40" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>90.82</v>
+        <v>100</v>
       </c>
       <c r="D40">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C42)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E40" s="33">
         <f>LN('Raw Data'!C42)</f>
         <v>4.3899948043230586</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" ht="15">
       <c r="A41" s="5">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -5091,18 +5181,18 @@
       </c>
       <c r="C41" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>33.35</v>
+        <v>46.82</v>
       </c>
       <c r="D41">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C43)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E41" s="33">
         <f>LN('Raw Data'!C43)</f>
         <v>4.5332444464165027</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" ht="15">
       <c r="A42" s="5">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -5112,18 +5202,18 @@
       </c>
       <c r="C42" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>37.869999999999997</v>
+        <v>63.96</v>
       </c>
       <c r="D42">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C44)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E42" s="33">
         <f>LN('Raw Data'!C44)</f>
         <v>2.0386195471595809</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" ht="15">
       <c r="A43" s="5">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -5133,18 +5223,18 @@
       </c>
       <c r="C43" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>77.819999999999993</v>
+        <v>53.81</v>
       </c>
       <c r="D43">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C45)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E43" s="33">
         <f>LN('Raw Data'!C45)</f>
         <v>3.2872818575322613</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" ht="15">
       <c r="A44" s="5">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -5154,18 +5244,18 @@
       </c>
       <c r="C44" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>62.54</v>
+        <v>53.83</v>
       </c>
       <c r="D44">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C46)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E44" s="33">
         <f>LN('Raw Data'!C46)</f>
         <v>4.2756934238792645</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" ht="15">
       <c r="A45" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -5175,18 +5265,18 @@
       </c>
       <c r="C45" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>29.48</v>
+        <v>88.95</v>
       </c>
       <c r="D45">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C47)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E45" s="33">
         <f>LN('Raw Data'!C47)</f>
         <v>3.7972853279577228</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" ht="15">
       <c r="A46" s="5">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -5196,18 +5286,18 @@
       </c>
       <c r="C46" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>25.48</v>
+        <v>22.58</v>
       </c>
       <c r="D46">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C48)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E46" s="33">
         <f>LN('Raw Data'!C48)</f>
         <v>3.9442965659784419</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" ht="15">
       <c r="A47" s="5">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -5217,18 +5307,18 @@
       </c>
       <c r="C47" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>48.86</v>
+        <v>27.23</v>
       </c>
       <c r="D47">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C49)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E47" s="33">
         <f>LN('Raw Data'!C49)</f>
         <v>4.3384665199215018</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" ht="15">
       <c r="A48" s="5">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -5238,18 +5328,18 @@
       </c>
       <c r="C48" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>41.96</v>
+        <v>68.55</v>
       </c>
       <c r="D48">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C50)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E48" s="33">
         <f>LN('Raw Data'!C50)</f>
         <v>4.6051701859880918</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" ht="15">
       <c r="A49" s="5">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -5259,18 +5349,18 @@
       </c>
       <c r="C49" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>49.06</v>
+        <v>100</v>
       </c>
       <c r="D49">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C51)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E49" s="33">
         <f>LN('Raw Data'!C51)</f>
         <v>3.8097687713893897</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" ht="15">
       <c r="A50" s="5">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -5280,18 +5370,18 @@
       </c>
       <c r="C50" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>72.11</v>
+        <v>83.35</v>
       </c>
       <c r="D50">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C52)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E50" s="33">
         <f>LN('Raw Data'!C52)</f>
         <v>4.0562964945845703</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" ht="15">
       <c r="A51" s="5">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -5301,18 +5391,18 @@
       </c>
       <c r="C51" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>58.2</v>
+        <v>84.06</v>
       </c>
       <c r="D51">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C53)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E51" s="33">
         <f>LN('Raw Data'!C53)</f>
         <v>4.5951198501345898</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" ht="15">
       <c r="A52" s="5">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -5322,18 +5412,18 @@
       </c>
       <c r="C52" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>41.66</v>
       </c>
       <c r="D52">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C54)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E52" s="33">
         <f>LN('Raw Data'!C54)</f>
         <v>3.6498787167642037</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" ht="15">
       <c r="A53" s="5">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -5343,18 +5433,18 @@
       </c>
       <c r="C53" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>94.56</v>
+        <v>43.67</v>
       </c>
       <c r="D53">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C55)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E53" s="33">
         <f>LN('Raw Data'!C55)</f>
         <v>3.6030491975087431</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" ht="15">
       <c r="A54" s="5">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -5364,11 +5454,11 @@
       </c>
       <c r="C54" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>48.4</v>
+        <v>43.38</v>
       </c>
       <c r="D54">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C56)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E54" s="33">
         <f>LN('Raw Data'!C56)</f>
@@ -5408,7 +5498,7 @@
       </c>
       <c r="B59" s="33">
         <f ca="1">AVERAGEA($C$3:$C$28)</f>
-        <v>61.86384615384614</v>
+        <v>58.589230769230774</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -5417,7 +5507,7 @@
       </c>
       <c r="B60" s="33">
         <f ca="1">AVERAGEA($C$29:$C$54)</f>
-        <v>58.960769230769223</v>
+        <v>64.220769230769235</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -5426,7 +5516,7 @@
       </c>
       <c r="B61" s="33">
         <f ca="1">STDEVA($C$3:$C$28)</f>
-        <v>22.045653009502519</v>
+        <v>21.184246962887656</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13">
@@ -5435,7 +5525,7 @@
       </c>
       <c r="B62" s="33">
         <f ca="1">STDEVA($C$29:$C$54)</f>
-        <v>21.749410092795983</v>
+        <v>23.803833627897301</v>
       </c>
     </row>
   </sheetData>
@@ -5525,7 +5615,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -5543,7 +5633,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -5561,7 +5651,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -5575,7 +5665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -5593,7 +5683,7 @@
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -5611,7 +5701,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -5629,7 +5719,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="21"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -5647,7 +5737,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -5664,7 +5754,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -5682,7 +5772,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -5698,7 +5788,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -5714,7 +5804,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -5728,7 +5818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -5742,7 +5832,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -5756,7 +5846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -5770,7 +5860,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -5784,7 +5874,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -5798,7 +5888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -5812,7 +5902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -5826,7 +5916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -5840,7 +5930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -5854,7 +5944,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -5868,7 +5958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -5882,7 +5972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -5896,7 +5986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -5910,7 +6000,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="15">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -5924,7 +6014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="15">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -5938,7 +6028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="15">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -5952,7 +6042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="15">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -5966,7 +6056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="15">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -5980,7 +6070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="15">
       <c r="A35" s="5">
         <v>31</v>
       </c>
@@ -5994,7 +6084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="15">
       <c r="A36" s="5">
         <v>32</v>
       </c>
@@ -6008,7 +6098,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="15">
       <c r="A37" s="5">
         <v>33</v>
       </c>
@@ -6022,7 +6112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" ht="15">
       <c r="A38" s="5">
         <v>34</v>
       </c>
@@ -6036,7 +6126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" ht="15">
       <c r="A39" s="5">
         <v>35</v>
       </c>
@@ -6050,7 +6140,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" ht="15">
       <c r="A40" s="5">
         <v>36</v>
       </c>
@@ -6064,7 +6154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" ht="15">
       <c r="A41" s="5">
         <v>37</v>
       </c>
@@ -6078,7 +6168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" ht="15">
       <c r="A42" s="5">
         <v>38</v>
       </c>
@@ -6092,7 +6182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" ht="15">
       <c r="A43" s="5">
         <v>39</v>
       </c>
@@ -6106,7 +6196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" ht="15">
       <c r="A44" s="5">
         <v>40</v>
       </c>
@@ -6120,7 +6210,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" ht="15">
       <c r="A45" s="5">
         <v>41</v>
       </c>
@@ -6134,7 +6224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" ht="15">
       <c r="A46" s="5">
         <v>42</v>
       </c>
@@ -6148,7 +6238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" ht="15">
       <c r="A47" s="5">
         <v>43</v>
       </c>
@@ -6162,7 +6252,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" ht="15">
       <c r="A48" s="5">
         <v>44</v>
       </c>
@@ -6176,7 +6266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" ht="15">
       <c r="A49" s="5">
         <v>45</v>
       </c>
@@ -6190,7 +6280,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" ht="15">
       <c r="A50" s="5">
         <v>46</v>
       </c>
@@ -6204,7 +6294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" ht="15">
       <c r="A51" s="5">
         <v>47</v>
       </c>
@@ -6218,7 +6308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" ht="15">
       <c r="A52" s="5">
         <v>48</v>
       </c>
@@ -6232,7 +6322,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" ht="15">
       <c r="A53" s="5">
         <v>49</v>
       </c>
@@ -6246,7 +6336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" ht="15">
       <c r="A54" s="5">
         <v>50</v>
       </c>
@@ -6260,7 +6350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" ht="15">
       <c r="A55" s="5">
         <v>51</v>
       </c>
@@ -6274,7 +6364,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" ht="15">
       <c r="A56" s="5">
         <v>52</v>
       </c>
@@ -6292,34 +6382,34 @@
       <c r="A58" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="95">
+      <c r="B58" s="96">
         <f>COUNTIF($B$5:$B$56, "Solo")</f>
         <v>26</v>
       </c>
-      <c r="C58" s="96"/>
-      <c r="D58" s="97"/>
+      <c r="C58" s="97"/>
+      <c r="D58" s="98"/>
     </row>
     <row r="59" spans="1:4" ht="13">
       <c r="A59" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="95">
+      <c r="B59" s="96">
         <f>COUNTIF($B$5:$B$56, "Pair")</f>
         <v>26</v>
       </c>
-      <c r="C59" s="96"/>
-      <c r="D59" s="97"/>
+      <c r="C59" s="97"/>
+      <c r="D59" s="98"/>
     </row>
     <row r="60" spans="1:4" ht="13">
       <c r="A60" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B60" s="95">
+      <c r="B60" s="96">
         <f>B58+2*B59</f>
         <v>78</v>
       </c>
-      <c r="C60" s="96"/>
-      <c r="D60" s="97"/>
+      <c r="C60" s="97"/>
+      <c r="D60" s="98"/>
     </row>
     <row r="98" spans="12:13" ht="13">
       <c r="L98" s="27" t="s">
@@ -6383,16 +6473,16 @@
     </row>
     <row r="2" spans="1:8" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="100" t="s">
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
     </row>
     <row r="3" spans="1:8" ht="13">
       <c r="A3" s="5"/>
@@ -7092,16 +7182,16 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="13">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="99"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
       </c>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
       <c r="F31" s="30">
         <f>COUNT(F$4:F$29)</f>
         <v>26</v>
@@ -7111,10 +7201,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A32" s="101" t="s">
+      <c r="A32" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="99"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="0">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -7137,10 +7227,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="13">
-      <c r="A33" s="101" t="s">
+      <c r="A33" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="99"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="32">
         <f>STDEV(C$4:C$29)</f>
         <v>18.729963016925137</v>
@@ -7160,10 +7250,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A34" s="101" t="s">
+      <c r="A34" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="99"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="3">SKEW(C$4:C$29)</f>
         <v>0.30912598517031509</v>
@@ -7183,10 +7273,10 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="13">
-      <c r="A35" s="101" t="s">
+      <c r="A35" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="99"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="5">MEDIAN(C$4:C$29)</f>
         <v>57.41</v>
@@ -7206,10 +7296,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="13">
-      <c r="A36" s="101" t="s">
+      <c r="A36" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="99"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="7">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -7229,10 +7319,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="13">
-      <c r="A37" s="101" t="s">
+      <c r="A37" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="99"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="9">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -7252,10 +7342,10 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="13">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="99"/>
+      <c r="B38" s="101"/>
       <c r="C38" s="34">
         <f t="shared" ref="C38:D38" si="11">QUARTILE(C$4:C$29, 1)</f>
         <v>51.019999999999996</v>
@@ -7275,10 +7365,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="13">
-      <c r="A39" s="101" t="s">
+      <c r="A39" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="99"/>
+      <c r="B39" s="101"/>
       <c r="C39" s="34">
         <f t="shared" ref="C39:D39" si="13">QUARTILE(C$4:C$29, 3)</f>
         <v>69.0625</v>
@@ -7298,10 +7388,10 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="13">
-      <c r="A40" s="101" t="s">
+      <c r="A40" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="99"/>
+      <c r="B40" s="101"/>
       <c r="C40" s="36">
         <f t="shared" ref="C40:D40" si="15">MAX(0, C38-1.5*(C39-C38))</f>
         <v>23.95624999999999</v>
@@ -7321,10 +7411,10 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="13">
-      <c r="A41" s="101" t="s">
+      <c r="A41" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="99"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="36">
         <f>MIN(C39+1.5*(C39-C38), 100)</f>
         <v>96.126249999999999</v>
@@ -7347,13 +7437,13 @@
       <c r="A43" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="102" t="s">
+      <c r="C43" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="99"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="99"/>
-      <c r="G43" s="99"/>
+      <c r="D43" s="101"/>
+      <c r="E43" s="101"/>
+      <c r="F43" s="101"/>
+      <c r="G43" s="101"/>
     </row>
     <row r="44" spans="1:9" ht="13">
       <c r="A44" s="39" t="s">
@@ -7373,12 +7463,12 @@
       <c r="E45" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="103" t="s">
+      <c r="F45" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="G45" s="96"/>
-      <c r="H45" s="96"/>
-      <c r="I45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="98"/>
     </row>
     <row r="46" spans="1:9" ht="13">
       <c r="A46" s="15" t="s">
@@ -7398,12 +7488,12 @@
       <c r="E46" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="104" t="s">
+      <c r="F46" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="96"/>
-      <c r="H46" s="96"/>
-      <c r="I46" s="97"/>
+      <c r="G46" s="97"/>
+      <c r="H46" s="97"/>
+      <c r="I46" s="98"/>
     </row>
     <row r="47" spans="1:9" ht="13">
       <c r="A47" s="15" t="s">
@@ -7423,12 +7513,12 @@
       <c r="E47" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F47" s="104" t="s">
+      <c r="F47" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="96"/>
-      <c r="H47" s="96"/>
-      <c r="I47" s="97"/>
+      <c r="G47" s="97"/>
+      <c r="H47" s="97"/>
+      <c r="I47" s="98"/>
     </row>
     <row r="48" spans="1:9" ht="13">
       <c r="A48" s="15" t="s">
@@ -7448,12 +7538,12 @@
       <c r="E48" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="104" t="s">
+      <c r="F48" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="G48" s="96"/>
-      <c r="H48" s="96"/>
-      <c r="I48" s="97"/>
+      <c r="G48" s="97"/>
+      <c r="H48" s="97"/>
+      <c r="I48" s="98"/>
     </row>
     <row r="49" spans="1:12" ht="13">
       <c r="A49" s="15" t="s">
@@ -7473,12 +7563,12 @@
       <c r="E49" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="104" t="s">
+      <c r="F49" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="G49" s="96"/>
-      <c r="H49" s="96"/>
-      <c r="I49" s="97"/>
+      <c r="G49" s="97"/>
+      <c r="H49" s="97"/>
+      <c r="I49" s="98"/>
     </row>
     <row r="50" spans="1:12" ht="13">
       <c r="A50" s="15" t="s">
@@ -7498,12 +7588,12 @@
       <c r="E50" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="104" t="s">
+      <c r="F50" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="G50" s="96"/>
-      <c r="H50" s="96"/>
-      <c r="I50" s="97"/>
+      <c r="G50" s="97"/>
+      <c r="H50" s="97"/>
+      <c r="I50" s="98"/>
     </row>
     <row r="51" spans="1:12" ht="13">
       <c r="B51" s="5" t="s">
@@ -7743,8 +7833,8 @@
       <c r="J85" s="41"/>
     </row>
     <row r="94" spans="9:12" ht="13">
-      <c r="I94" s="105"/>
-      <c r="J94" s="99"/>
+      <c r="I94" s="100"/>
+      <c r="J94" s="101"/>
     </row>
     <row r="95" spans="9:12" ht="13">
       <c r="I95" s="4"/>
@@ -7752,11 +7842,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C43:G43"/>
@@ -7769,11 +7859,11 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="I94:J94"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C29">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
@@ -7946,10 +8036,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="268" zoomScaleNormal="268" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7968,7 +8058,7 @@
     <col min="14" max="14" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1">
       <c r="B1" s="42" t="s">
         <v>43</v>
       </c>
@@ -7981,7 +8071,7 @@
       <c r="M1" s="43"/>
       <c r="N1" s="43"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1">
       <c r="B2" s="42"/>
       <c r="C2" s="5"/>
       <c r="E2" s="5"/>
@@ -7992,7 +8082,7 @@
       <c r="M2" s="43"/>
       <c r="N2" s="43"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1">
       <c r="B3" s="44"/>
       <c r="C3" s="5"/>
       <c r="E3" s="5"/>
@@ -8002,15 +8092,15 @@
       <c r="H3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="106" t="s">
+      <c r="J3" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="45" t="str">
         <f>'Raw Data'!A4</f>
         <v>Case #</v>
@@ -8029,17 +8119,17 @@
       <c r="E4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="107" t="s">
+      <c r="G4" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="99"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H4" s="101"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5">
         <f>'Raw Data'!A5</f>
         <v>1</v>
@@ -8067,13 +8157,25 @@
         <f>PEARSON($B$5:$B$56, $D$5:$D$56)</f>
         <v>-0.91720677499078029</v>
       </c>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
+      <c r="P5" s="95">
+        <f>PEARSON($D$5:$D$56, $B$5:$B$56)</f>
+        <v>-0.91720677499078029</v>
+      </c>
+      <c r="Q5">
+        <f>CORREL($B$5:$B$56, $D$5:$D$56)</f>
+        <v>-0.91720677499078029</v>
+      </c>
+      <c r="R5">
+        <f>CORREL($B$5:$B$56, $D$5:$D$56)</f>
+        <v>-0.91720677499078029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6">
         <f>'Raw Data'!A6</f>
         <v>2</v>
@@ -8101,13 +8203,25 @@
         <f>PEARSON($C$5:C$56, $E$5:E$56)</f>
         <v>-0.8811057107791842</v>
       </c>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
-      <c r="N6" s="99"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="101"/>
+      <c r="N6" s="101"/>
+      <c r="P6" s="95">
+        <f>PEARSON($E$5:E$56, $C$5:C$56)</f>
+        <v>-0.8811057107791842</v>
+      </c>
+      <c r="Q6">
+        <f>CORREL($C$5:C$56, $E$5:E$56)</f>
+        <v>-0.8811057107791842</v>
+      </c>
+      <c r="R6" s="95">
+        <f>CORREL($E$5:E$56, $C$5:C$56)</f>
+        <v>-0.8811057107791842</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1">
       <c r="A7">
         <f>'Raw Data'!A7</f>
         <v>3</v>
@@ -8128,13 +8242,13 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="101"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8">
         <f>'Raw Data'!A8</f>
         <v>4</v>
@@ -8158,13 +8272,13 @@
       <c r="G8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="99"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9">
         <f>'Raw Data'!A9</f>
         <v>5</v>
@@ -8192,13 +8306,13 @@
         <f>INTERCEPT($D$5:$D$56, $B$5:$B$56)</f>
         <v>46.129734040658491</v>
       </c>
-      <c r="J9" s="99"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="99"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="101"/>
+      <c r="N9" s="101"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10">
         <f>'Raw Data'!A10</f>
         <v>6</v>
@@ -8226,13 +8340,13 @@
         <f>SLOPE($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.3967422303778369</v>
       </c>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="99"/>
-      <c r="N10" s="99"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J10" s="101"/>
+      <c r="K10" s="101"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+      <c r="N10" s="101"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11">
         <f>'Raw Data'!A11</f>
         <v>7</v>
@@ -8260,13 +8374,13 @@
         <v>56</v>
       </c>
       <c r="I11" s="50"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="99"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J11" s="101"/>
+      <c r="K11" s="101"/>
+      <c r="L11" s="101"/>
+      <c r="M11" s="101"/>
+      <c r="N11" s="101"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12">
         <f>'Raw Data'!A12</f>
         <v>8</v>
@@ -8294,13 +8408,13 @@
         <v>58</v>
       </c>
       <c r="I12" s="50"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="99"/>
-      <c r="N12" s="99"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -8327,13 +8441,13 @@
         <f>D58*SQRT((1-H5^2)*((B59-1)/(B59-2)))</f>
         <v>3.6418560620845599</v>
       </c>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J13" s="101"/>
+      <c r="K13" s="101"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="101"/>
+      <c r="N13" s="101"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14">
         <f>'Raw Data'!A14</f>
         <v>10</v>
@@ -8361,13 +8475,13 @@
         <f>H13/(B58*SQRT(B59-1))</f>
         <v>2.4599907197583686E-2</v>
       </c>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="99"/>
-      <c r="M14" s="99"/>
-      <c r="N14" s="99"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="101"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15">
         <f>'Raw Data'!A15</f>
         <v>11</v>
@@ -8395,13 +8509,13 @@
         <f>H10/H14</f>
         <v>-16.127793783580074</v>
       </c>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1">
+      <c r="J15" s="101"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="101"/>
+      <c r="M15" s="101"/>
+      <c r="N15" s="101"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1">
       <c r="A16">
         <f>'Raw Data'!A16</f>
         <v>12</v>
@@ -8432,11 +8546,11 @@
       <c r="I16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+      <c r="N16" s="101"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17">
@@ -8645,7 +8759,7 @@
         <f>IF(OR(0&lt;H21, 0&gt;H22), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="I23" s="109" t="s">
+      <c r="I23" s="119" t="s">
         <v>74</v>
       </c>
       <c r="J23" s="45"/>
@@ -8678,7 +8792,7 @@
         <f>IF(ABS(H15)&gt;H20, "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="I24" s="99"/>
+      <c r="I24" s="101"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25">
@@ -8835,12 +8949,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G29" s="101" t="s">
+      <c r="G29" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
       <c r="K29" s="64">
         <f>H9+H10*15</f>
         <v>40.178600584990939</v>
@@ -8895,11 +9009,11 @@
       <c r="G31" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="H31" s="110" t="s">
+      <c r="H31" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="I31" s="111"/>
-      <c r="J31" s="112"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="109"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1">
       <c r="A32">
@@ -8922,12 +9036,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="G32" s="118" t="s">
+      <c r="G32" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="113"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="114"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="101"/>
+      <c r="J32" s="111"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
       <c r="A33">
@@ -8950,10 +9064,10 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="G33" s="99"/>
-      <c r="H33" s="113"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="114"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="111"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34">
@@ -8976,10 +9090,10 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="G34" s="99"/>
-      <c r="H34" s="113"/>
-      <c r="I34" s="99"/>
-      <c r="J34" s="114"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="110"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="111"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1">
       <c r="A35">
@@ -9002,10 +9116,10 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="G35" s="99"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="114"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="110"/>
+      <c r="I35" s="101"/>
+      <c r="J35" s="111"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
       <c r="A36">
@@ -9028,9 +9142,9 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H36" s="113"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="114"/>
+      <c r="H36" s="110"/>
+      <c r="I36" s="101"/>
+      <c r="J36" s="111"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
       <c r="A37">
@@ -9053,9 +9167,9 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="H37" s="115"/>
-      <c r="I37" s="116"/>
-      <c r="J37" s="117"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="114"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38">
@@ -9636,11 +9750,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="45"/>
@@ -9660,13 +9774,13 @@
       <c r="C4" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="124" t="s">
+      <c r="D4" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="98"/>
       <c r="I4" s="69"/>
       <c r="J4" s="69"/>
     </row>
@@ -9726,14 +9840,14 @@
       <c r="C8" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="124" t="str">
+      <c r="D8" s="122" t="str">
         <f>D4</f>
         <v>quality difference between solo and pair programmers.</v>
       </c>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="98"/>
       <c r="I8" s="69"/>
       <c r="J8" s="69"/>
     </row>
@@ -9779,13 +9893,13 @@
       <c r="C13" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="118" t="s">
+      <c r="D13" s="115" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
@@ -9819,17 +9933,17 @@
       <c r="C16" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="125" t="s">
+      <c r="D16" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="104" t="s">
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="97"/>
+      <c r="J16" s="98"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="15"/>
@@ -9842,27 +9956,27 @@
       <c r="B18" s="120" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="97"/>
+      <c r="C18" s="98"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="119">
+      <c r="B19" s="124">
         <f>TTEST('Data Transformation'!C4:C29, 'Data Transformation'!F4:F29, 2, 2)</f>
         <v>0.86409838706386388</v>
       </c>
-      <c r="C19" s="97"/>
+      <c r="C19" s="98"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="103">
+      <c r="B20" s="104">
         <v>0.05</v>
       </c>
-      <c r="C20" s="97"/>
+      <c r="C20" s="98"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15" t="s">
@@ -9871,7 +9985,7 @@
       <c r="B21" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="97"/>
+      <c r="C21" s="98"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="45"/>
@@ -9909,11 +10023,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="15">
       <c r="A27" s="45"/>
       <c r="E27" s="77"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="15">
       <c r="A28" s="15" t="s">
         <v>123</v>
       </c>
@@ -9921,7 +10035,7 @@
         <f>1-B19</f>
         <v>0.13590161293613612</v>
       </c>
-      <c r="C28" s="121" t="s">
+      <c r="C28" s="125" t="s">
         <v>124</v>
       </c>
       <c r="D28" s="79" t="s">
@@ -9936,7 +10050,7 @@
         <f>'Data Transformation'!C31+'Data Transformation'!F31-2</f>
         <v>50</v>
       </c>
-      <c r="C29" s="99"/>
+      <c r="C29" s="101"/>
       <c r="D29" s="5" t="s">
         <v>126</v>
       </c>
@@ -9949,7 +10063,7 @@
         <f>TINV(B19,B29)</f>
         <v>0.17204274843003223</v>
       </c>
-      <c r="C30" s="99"/>
+      <c r="C30" s="101"/>
       <c r="D30" s="5" t="s">
         <v>128</v>
       </c>
@@ -9962,7 +10076,7 @@
         <f>B23-'Data Transformation'!C42*B30</f>
         <v>2.9154700840650083E-3</v>
       </c>
-      <c r="C31" s="99"/>
+      <c r="C31" s="101"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15" t="s">
@@ -9972,7 +10086,7 @@
         <f>B23+'Data Transformation'!C42*B30</f>
         <v>1.997084529915935</v>
       </c>
-      <c r="C32" s="99"/>
+      <c r="C32" s="101"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="50"/>
@@ -9999,11 +10113,11 @@
       <c r="G35" s="67"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A36" s="122" t="s">
+      <c r="A36" s="126" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="116"/>
-      <c r="C36" s="116"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="113"/>
       <c r="D36" s="83">
         <f>B31</f>
         <v>2.9154700840650083E-3</v>
@@ -10023,79 +10137,79 @@
       <c r="A38" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="123" t="s">
+      <c r="B38" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="111"/>
-      <c r="D38" s="112"/>
+      <c r="C38" s="108"/>
+      <c r="D38" s="109"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B39" s="113"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="114"/>
+      <c r="B39" s="110"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="111"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B40" s="113"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="114"/>
+      <c r="B40" s="110"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="111"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B41" s="113"/>
-      <c r="C41" s="99"/>
-      <c r="D41" s="114"/>
+      <c r="B41" s="110"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="111"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B42" s="113"/>
-      <c r="C42" s="99"/>
-      <c r="D42" s="114"/>
+      <c r="B42" s="110"/>
+      <c r="C42" s="101"/>
+      <c r="D42" s="111"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="45"/>
-      <c r="B43" s="113"/>
-      <c r="C43" s="99"/>
-      <c r="D43" s="114"/>
+      <c r="B43" s="110"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="111"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
       <c r="A44" s="45"/>
-      <c r="B44" s="113"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="114"/>
+      <c r="B44" s="110"/>
+      <c r="C44" s="101"/>
+      <c r="D44" s="111"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
       <c r="A45" s="45"/>
-      <c r="B45" s="113"/>
-      <c r="C45" s="99"/>
-      <c r="D45" s="114"/>
+      <c r="B45" s="110"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="111"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
       <c r="A46" s="45"/>
-      <c r="B46" s="113"/>
-      <c r="C46" s="99"/>
-      <c r="D46" s="114"/>
+      <c r="B46" s="110"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="111"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
       <c r="A47" s="45"/>
-      <c r="B47" s="113"/>
-      <c r="C47" s="99"/>
-      <c r="D47" s="114"/>
+      <c r="B47" s="110"/>
+      <c r="C47" s="101"/>
+      <c r="D47" s="111"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
       <c r="A48" s="45"/>
-      <c r="B48" s="113"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="114"/>
+      <c r="B48" s="110"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="111"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="45"/>
-      <c r="B49" s="113"/>
-      <c r="C49" s="99"/>
-      <c r="D49" s="114"/>
+      <c r="B49" s="110"/>
+      <c r="C49" s="101"/>
+      <c r="D49" s="111"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="45"/>
-      <c r="B50" s="115"/>
-      <c r="C50" s="116"/>
-      <c r="D50" s="117"/>
+      <c r="B50" s="112"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="114"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="45"/>

</xml_diff>

<commit_message>
Update A1_Solution's Relationships alternative cells to have proper value
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB4F613-709B-4949-88D8-D3A8C653FCA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DD8430-3295-974E-B1AB-7264A8A60046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="15740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,15 +388,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> - R5</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> - R5
 </t>
         </r>
         <r>
@@ -448,15 +440,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>alt_cells:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">alt_cells:
 </t>
         </r>
         <r>
@@ -465,15 +449,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> - P5</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> - P6
 </t>
         </r>
         <r>
@@ -482,15 +458,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> - Q5</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> - Q6
 </t>
         </r>
         <r>
@@ -499,7 +467,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> - R5</t>
+          <t xml:space="preserve"> - R6</t>
         </r>
         <r>
           <rPr>
@@ -1903,20 +1871,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3122,16 +3090,16 @@
     </row>
     <row r="2" spans="1:10" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="106" t="s">
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="I2" s="127" t="s">
         <v>135</v>
       </c>
@@ -3874,23 +3842,23 @@
         <v>4.0055133485154846</v>
       </c>
       <c r="H29" s="4"/>
-      <c r="I29" s="100"/>
-      <c r="J29" s="101"/>
-      <c r="K29" s="101"/>
-      <c r="L29" s="101"/>
+      <c r="I29" s="106"/>
+      <c r="J29" s="100"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="100"/>
     </row>
     <row r="30" spans="1:12" ht="13">
       <c r="H30" s="4"/>
-      <c r="I30" s="100"/>
-      <c r="J30" s="101"/>
-      <c r="K30" s="100"/>
-      <c r="L30" s="101"/>
+      <c r="I30" s="106"/>
+      <c r="J30" s="100"/>
+      <c r="K30" s="106"/>
+      <c r="L30" s="100"/>
     </row>
     <row r="31" spans="1:12" ht="13">
       <c r="A31" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="101"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
@@ -3909,7 +3877,7 @@
       <c r="A32" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="101"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="2">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -3933,13 +3901,13 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="101"/>
+      <c r="L32" s="100"/>
     </row>
     <row r="33" spans="1:12" ht="13">
       <c r="A33" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="101"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="32">
         <f t="shared" ref="C33:D33" si="4">STDEVA(C$4:C$11, C$13:C$29)</f>
         <v>18.592928377925453</v>
@@ -3963,13 +3931,13 @@
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="101"/>
+      <c r="L33" s="100"/>
     </row>
     <row r="34" spans="1:12" ht="17.25" customHeight="1">
       <c r="A34" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="101"/>
+      <c r="B34" s="100"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="6">SKEW(C$4:C$11, C$13:C$29)</f>
         <v>0.24893711104029126</v>
@@ -3991,13 +3959,13 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="101"/>
+      <c r="L34" s="100"/>
     </row>
     <row r="35" spans="1:12" ht="13">
       <c r="A35" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="101"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="8">MEDIAN(C$4:C$11, C$13:C$29)</f>
         <v>57.68</v>
@@ -4021,13 +3989,13 @@
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="101"/>
+      <c r="L35" s="100"/>
     </row>
     <row r="36" spans="1:12" ht="13">
       <c r="A36" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="101"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="10">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -4052,13 +4020,13 @@
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="101"/>
+      <c r="L36" s="100"/>
     </row>
     <row r="37" spans="1:12" ht="13">
       <c r="A37" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="101"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="12">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -4080,7 +4048,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="101"/>
+      <c r="L37" s="100"/>
     </row>
     <row r="38" spans="1:12" ht="13">
       <c r="A38" s="15"/>
@@ -4093,7 +4061,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="101"/>
+      <c r="L38" s="100"/>
     </row>
     <row r="39" spans="1:12" ht="13">
       <c r="A39" s="15"/>
@@ -4111,13 +4079,13 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="101"/>
+      <c r="L39" s="100"/>
     </row>
     <row r="40" spans="1:12" ht="15">
       <c r="A40" s="102" t="s">
         <v>138</v>
       </c>
-      <c r="B40" s="101"/>
+      <c r="B40" s="100"/>
       <c r="C40" s="51">
         <f>SQRT((C33^2*(C31-1)+F33^2*(F31-1))/(C31+F31-2))</f>
         <v>20.89619836575601</v>
@@ -4133,13 +4101,13 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="101"/>
+      <c r="L40" s="100"/>
     </row>
     <row r="41" spans="1:12" ht="15">
       <c r="A41" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="101"/>
+      <c r="B41" s="100"/>
       <c r="C41" s="32">
         <f t="shared" ref="C41:D41" si="14">ABS(C32-F32)</f>
         <v>1</v>
@@ -4158,7 +4126,7 @@
       <c r="A42" s="102" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="101"/>
+      <c r="B42" s="100"/>
       <c r="C42" s="32">
         <f t="shared" ref="C42:D42" si="15">SQRT(C33^2/$C31 + F33^2/$F31)</f>
         <v>5.7955626669230851</v>
@@ -4188,16 +4156,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J22"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="L32:L40"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
@@ -4206,6 +4164,16 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="L32:L40"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J22"/>
+    <mergeCell ref="I29:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4285,7 +4253,7 @@
       </c>
       <c r="C3" s="94">
         <f t="shared" ref="C3:C28" ca="1" si="0">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$3, $I$3)),0), 2)</f>
-        <v>55.03</v>
+        <v>44.25</v>
       </c>
       <c r="D3">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C5)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4321,11 +4289,11 @@
       </c>
       <c r="C4" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>7.29</v>
+        <v>29.29</v>
       </c>
       <c r="D4">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C6)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E4" s="33">
         <f>LN('Raw Data'!C6)</f>
@@ -4346,11 +4314,11 @@
       </c>
       <c r="C5" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>38.53</v>
+        <v>52.92</v>
       </c>
       <c r="D5">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C7)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="33">
         <f>LN('Raw Data'!C7)</f>
@@ -4367,11 +4335,11 @@
       </c>
       <c r="C6" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>32.21</v>
+        <v>65.75</v>
       </c>
       <c r="D6">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C8)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E6" s="33">
         <f>LN('Raw Data'!C8)</f>
@@ -4400,11 +4368,11 @@
       </c>
       <c r="C7" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>67.91</v>
+        <v>48.31</v>
       </c>
       <c r="D7">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C9)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="33">
         <f>LN('Raw Data'!C9)</f>
@@ -4434,11 +4402,11 @@
       </c>
       <c r="C8" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>46.26</v>
       </c>
       <c r="D8">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C10)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="33">
         <f>LN('Raw Data'!C10)</f>
@@ -4470,11 +4438,11 @@
       </c>
       <c r="C9" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>67.84</v>
+        <v>74.94</v>
       </c>
       <c r="D9">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C11)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E9" s="33">
         <f>LN('Raw Data'!C11)</f>
@@ -4495,11 +4463,11 @@
       </c>
       <c r="C10" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>35.92</v>
+        <v>11.48</v>
       </c>
       <c r="D10">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C12)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E10" s="33">
         <f>LN('Raw Data'!C12)</f>
@@ -4526,11 +4494,11 @@
       </c>
       <c r="C11" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>45.67</v>
+        <v>23.97</v>
       </c>
       <c r="D11">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C13)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E11" s="33">
         <f>LN('Raw Data'!C13)</f>
@@ -4558,11 +4526,11 @@
       </c>
       <c r="C12" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>68.349999999999994</v>
+        <v>64.349999999999994</v>
       </c>
       <c r="D12">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C14)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E12" s="33">
         <f>LN('Raw Data'!C14)</f>
@@ -4586,11 +4554,11 @@
       </c>
       <c r="C13" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>65.650000000000006</v>
+        <v>82.71</v>
       </c>
       <c r="D13">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C15)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="33">
         <f>LN('Raw Data'!C15)</f>
@@ -4614,11 +4582,11 @@
       </c>
       <c r="C14" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>63.33</v>
+        <v>16.440000000000001</v>
       </c>
       <c r="D14">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C16)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="33">
         <f>LN('Raw Data'!C16)</f>
@@ -4635,11 +4603,11 @@
       </c>
       <c r="C15" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>67.94</v>
+        <v>100</v>
       </c>
       <c r="D15">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C17)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="33">
         <f>LN('Raw Data'!C17)</f>
@@ -4656,11 +4624,11 @@
       </c>
       <c r="C16" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>80.05</v>
+        <v>55</v>
       </c>
       <c r="D16">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C18)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E16" s="33">
         <f>LN('Raw Data'!C18)</f>
@@ -4677,11 +4645,11 @@
       </c>
       <c r="C17" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>56.11</v>
+        <v>35.9</v>
       </c>
       <c r="D17">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C19)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E17" s="33">
         <f>LN('Raw Data'!C19)</f>
@@ -4698,11 +4666,11 @@
       </c>
       <c r="C18" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>86.35</v>
+        <v>58.08</v>
       </c>
       <c r="D18">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C20)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="33">
         <f>LN('Raw Data'!C20)</f>
@@ -4719,11 +4687,11 @@
       </c>
       <c r="C19" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>66.05</v>
+        <v>76.94</v>
       </c>
       <c r="D19">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C21)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E19" s="33">
         <f>LN('Raw Data'!C21)</f>
@@ -4740,7 +4708,7 @@
       </c>
       <c r="C20" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>64.069999999999993</v>
+        <v>53.35</v>
       </c>
       <c r="D20">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C22)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4761,11 +4729,11 @@
       </c>
       <c r="C21" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>61.25</v>
+        <v>97.21</v>
       </c>
       <c r="D21">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C23)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E21" s="33">
         <f>LN('Raw Data'!C23)</f>
@@ -4782,11 +4750,11 @@
       </c>
       <c r="C22" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>72.12</v>
+        <v>65.7</v>
       </c>
       <c r="D22">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C24)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E22" s="33">
         <f>LN('Raw Data'!C24)</f>
@@ -4803,11 +4771,11 @@
       </c>
       <c r="C23" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>87.71</v>
+        <v>70.319999999999993</v>
       </c>
       <c r="D23">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C25)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E23" s="33">
         <f>LN('Raw Data'!C25)</f>
@@ -4824,11 +4792,11 @@
       </c>
       <c r="C24" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>57.22</v>
+        <v>61.78</v>
       </c>
       <c r="D24">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C26)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E24" s="33">
         <f>LN('Raw Data'!C26)</f>
@@ -4845,11 +4813,11 @@
       </c>
       <c r="C25" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>68.900000000000006</v>
+        <v>38.020000000000003</v>
       </c>
       <c r="D25">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C27)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E25" s="33">
         <f>LN('Raw Data'!C27)</f>
@@ -4866,11 +4834,11 @@
       </c>
       <c r="C26" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>54.44</v>
+        <v>96.69</v>
       </c>
       <c r="D26">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C28)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E26" s="33">
         <f>LN('Raw Data'!C28)</f>
@@ -4887,11 +4855,11 @@
       </c>
       <c r="C27" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>18.57</v>
+        <v>25.47</v>
       </c>
       <c r="D27">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C29)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27" s="33">
         <f>LN('Raw Data'!C29)</f>
@@ -4908,11 +4876,11 @@
       </c>
       <c r="C28" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>34.81</v>
+        <v>94.5</v>
       </c>
       <c r="D28">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C30)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E28" s="33">
         <f>LN('Raw Data'!C30)</f>
@@ -4929,11 +4897,11 @@
       </c>
       <c r="C29" s="94">
         <f t="shared" ref="C29:C54" ca="1" si="2">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$8, $I$8)),0), 2)</f>
-        <v>96.19</v>
+        <v>77.41</v>
       </c>
       <c r="D29">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C31)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29" s="33">
         <f>LN('Raw Data'!C31)</f>
@@ -4950,7 +4918,7 @@
       </c>
       <c r="C30" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>42.38</v>
+        <v>21.79</v>
       </c>
       <c r="D30">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C32)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4971,11 +4939,11 @@
       </c>
       <c r="C31" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>72.56</v>
+        <v>90.58</v>
       </c>
       <c r="D31">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C33)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E31" s="33">
         <f>LN('Raw Data'!C33)</f>
@@ -4992,7 +4960,7 @@
       </c>
       <c r="C32" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>37.950000000000003</v>
+        <v>16.239999999999998</v>
       </c>
       <c r="D32">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C34)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -5013,11 +4981,11 @@
       </c>
       <c r="C33" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>60.98</v>
+        <v>79.72</v>
       </c>
       <c r="D33">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C35)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E33" s="33">
         <f>LN('Raw Data'!C35)</f>
@@ -5034,11 +5002,11 @@
       </c>
       <c r="C34" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>68.41</v>
       </c>
       <c r="D34">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C36)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E34" s="33">
         <f>LN('Raw Data'!C36)</f>
@@ -5055,11 +5023,11 @@
       </c>
       <c r="C35" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>54.47</v>
+        <v>94.4</v>
       </c>
       <c r="D35">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C37)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E35" s="33">
         <f>LN('Raw Data'!C37)</f>
@@ -5076,11 +5044,11 @@
       </c>
       <c r="C36" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>54.01</v>
+        <v>60.39</v>
       </c>
       <c r="D36">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C38)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E36" s="33">
         <f>LN('Raw Data'!C38)</f>
@@ -5097,11 +5065,11 @@
       </c>
       <c r="C37" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>54.55</v>
+        <v>59.87</v>
       </c>
       <c r="D37">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C39)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E37" s="33">
         <f>LN('Raw Data'!C39)</f>
@@ -5118,11 +5086,11 @@
       </c>
       <c r="C38" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>99.88</v>
+        <v>84.25</v>
       </c>
       <c r="D38">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C40)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E38" s="33">
         <f>LN('Raw Data'!C40)</f>
@@ -5139,11 +5107,11 @@
       </c>
       <c r="C39" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>74.92</v>
+        <v>25.42</v>
       </c>
       <c r="D39">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C41)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E39" s="33">
         <f>LN('Raw Data'!C41)</f>
@@ -5164,7 +5132,7 @@
       </c>
       <c r="D40">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C42)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E40" s="33">
         <f>LN('Raw Data'!C42)</f>
@@ -5181,11 +5149,11 @@
       </c>
       <c r="C41" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>46.82</v>
+        <v>71.09</v>
       </c>
       <c r="D41">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C43)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E41" s="33">
         <f>LN('Raw Data'!C43)</f>
@@ -5202,11 +5170,11 @@
       </c>
       <c r="C42" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>63.96</v>
+        <v>65.58</v>
       </c>
       <c r="D42">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C44)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E42" s="33">
         <f>LN('Raw Data'!C44)</f>
@@ -5223,11 +5191,11 @@
       </c>
       <c r="C43" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>53.81</v>
+        <v>94.62</v>
       </c>
       <c r="D43">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C45)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E43" s="33">
         <f>LN('Raw Data'!C45)</f>
@@ -5244,11 +5212,11 @@
       </c>
       <c r="C44" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>53.83</v>
+        <v>40.729999999999997</v>
       </c>
       <c r="D44">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C46)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E44" s="33">
         <f>LN('Raw Data'!C46)</f>
@@ -5265,11 +5233,11 @@
       </c>
       <c r="C45" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>88.95</v>
+        <v>37.75</v>
       </c>
       <c r="D45">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C47)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E45" s="33">
         <f>LN('Raw Data'!C47)</f>
@@ -5286,11 +5254,11 @@
       </c>
       <c r="C46" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>22.58</v>
+        <v>69.239999999999995</v>
       </c>
       <c r="D46">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C48)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E46" s="33">
         <f>LN('Raw Data'!C48)</f>
@@ -5307,11 +5275,11 @@
       </c>
       <c r="C47" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>27.23</v>
+        <v>20.61</v>
       </c>
       <c r="D47">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C49)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E47" s="33">
         <f>LN('Raw Data'!C49)</f>
@@ -5328,11 +5296,11 @@
       </c>
       <c r="C48" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>68.55</v>
+        <v>63.58</v>
       </c>
       <c r="D48">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C50)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" s="33">
         <f>LN('Raw Data'!C50)</f>
@@ -5349,11 +5317,11 @@
       </c>
       <c r="C49" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>88.46</v>
       </c>
       <c r="D49">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C51)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E49" s="33">
         <f>LN('Raw Data'!C51)</f>
@@ -5370,11 +5338,11 @@
       </c>
       <c r="C50" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>83.35</v>
+        <v>47.6</v>
       </c>
       <c r="D50">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C52)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E50" s="33">
         <f>LN('Raw Data'!C52)</f>
@@ -5391,11 +5359,11 @@
       </c>
       <c r="C51" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>84.06</v>
+        <v>64.510000000000005</v>
       </c>
       <c r="D51">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C53)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E51" s="33">
         <f>LN('Raw Data'!C53)</f>
@@ -5412,11 +5380,11 @@
       </c>
       <c r="C52" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>41.66</v>
+        <v>37.71</v>
       </c>
       <c r="D52">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C54)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E52" s="33">
         <f>LN('Raw Data'!C54)</f>
@@ -5433,11 +5401,11 @@
       </c>
       <c r="C53" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>43.67</v>
+        <v>79.36</v>
       </c>
       <c r="D53">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C55)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E53" s="33">
         <f>LN('Raw Data'!C55)</f>
@@ -5454,11 +5422,11 @@
       </c>
       <c r="C54" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>43.38</v>
+        <v>62.32</v>
       </c>
       <c r="D54">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C56)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E54" s="33">
         <f>LN('Raw Data'!C56)</f>
@@ -5498,7 +5466,7 @@
       </c>
       <c r="B59" s="33">
         <f ca="1">AVERAGEA($C$3:$C$28)</f>
-        <v>58.589230769230774</v>
+        <v>57.293461538461543</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -5507,7 +5475,7 @@
       </c>
       <c r="B60" s="33">
         <f ca="1">AVERAGEA($C$29:$C$54)</f>
-        <v>64.220769230769235</v>
+        <v>62.37076923076922</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -5516,7 +5484,7 @@
       </c>
       <c r="B61" s="33">
         <f ca="1">STDEVA($C$3:$C$28)</f>
-        <v>21.184246962887656</v>
+        <v>25.295303902868234</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13">
@@ -5525,7 +5493,7 @@
       </c>
       <c r="B62" s="33">
         <f ca="1">STDEVA($C$29:$C$54)</f>
-        <v>23.803833627897301</v>
+        <v>24.67708620126405</v>
       </c>
     </row>
   </sheetData>
@@ -6473,16 +6441,16 @@
     </row>
     <row r="2" spans="1:8" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="106" t="s">
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
     </row>
     <row r="3" spans="1:8" ht="13">
       <c r="A3" s="5"/>
@@ -7185,13 +7153,13 @@
       <c r="A31" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="101"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
       </c>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
       <c r="F31" s="30">
         <f>COUNT(F$4:F$29)</f>
         <v>26</v>
@@ -7204,7 +7172,7 @@
       <c r="A32" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="101"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="0">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -7230,7 +7198,7 @@
       <c r="A33" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="101"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="32">
         <f>STDEV(C$4:C$29)</f>
         <v>18.729963016925137</v>
@@ -7253,7 +7221,7 @@
       <c r="A34" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="101"/>
+      <c r="B34" s="100"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="3">SKEW(C$4:C$29)</f>
         <v>0.30912598517031509</v>
@@ -7276,7 +7244,7 @@
       <c r="A35" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="101"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="5">MEDIAN(C$4:C$29)</f>
         <v>57.41</v>
@@ -7299,7 +7267,7 @@
       <c r="A36" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="101"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="7">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -7322,7 +7290,7 @@
       <c r="A37" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="101"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="9">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -7345,7 +7313,7 @@
       <c r="A38" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="34">
         <f t="shared" ref="C38:D38" si="11">QUARTILE(C$4:C$29, 1)</f>
         <v>51.019999999999996</v>
@@ -7368,7 +7336,7 @@
       <c r="A39" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="101"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="34">
         <f t="shared" ref="C39:D39" si="13">QUARTILE(C$4:C$29, 3)</f>
         <v>69.0625</v>
@@ -7391,7 +7359,7 @@
       <c r="A40" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="101"/>
+      <c r="B40" s="100"/>
       <c r="C40" s="36">
         <f t="shared" ref="C40:D40" si="15">MAX(0, C38-1.5*(C39-C38))</f>
         <v>23.95624999999999</v>
@@ -7414,7 +7382,7 @@
       <c r="A41" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="101"/>
+      <c r="B41" s="100"/>
       <c r="C41" s="36">
         <f>MIN(C39+1.5*(C39-C38), 100)</f>
         <v>96.126249999999999</v>
@@ -7440,10 +7408,10 @@
       <c r="C43" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="101"/>
-      <c r="E43" s="101"/>
-      <c r="F43" s="101"/>
-      <c r="G43" s="101"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="100"/>
+      <c r="G43" s="100"/>
     </row>
     <row r="44" spans="1:9" ht="13">
       <c r="A44" s="39" t="s">
@@ -7488,7 +7456,7 @@
       <c r="E46" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="99" t="s">
+      <c r="F46" s="105" t="s">
         <v>36</v>
       </c>
       <c r="G46" s="97"/>
@@ -7513,7 +7481,7 @@
       <c r="E47" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F47" s="99" t="s">
+      <c r="F47" s="105" t="s">
         <v>36</v>
       </c>
       <c r="G47" s="97"/>
@@ -7538,7 +7506,7 @@
       <c r="E48" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="99" t="s">
+      <c r="F48" s="105" t="s">
         <v>36</v>
       </c>
       <c r="G48" s="97"/>
@@ -7563,7 +7531,7 @@
       <c r="E49" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="99" t="s">
+      <c r="F49" s="105" t="s">
         <v>36</v>
       </c>
       <c r="G49" s="97"/>
@@ -7588,7 +7556,7 @@
       <c r="E50" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="99" t="s">
+      <c r="F50" s="105" t="s">
         <v>36</v>
       </c>
       <c r="G50" s="97"/>
@@ -7833,8 +7801,8 @@
       <c r="J85" s="41"/>
     </row>
     <row r="94" spans="9:12" ht="13">
-      <c r="I94" s="100"/>
-      <c r="J94" s="101"/>
+      <c r="I94" s="106"/>
+      <c r="J94" s="100"/>
     </row>
     <row r="95" spans="9:12" ht="13">
       <c r="I95" s="4"/>
@@ -7842,11 +7810,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="I94:J94"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C43:G43"/>
@@ -7859,11 +7827,11 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C29">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
@@ -8038,8 +8006,8 @@
   </sheetPr>
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -8095,10 +8063,10 @@
       <c r="J3" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="45" t="str">
@@ -8122,12 +8090,12 @@
       <c r="G4" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="101"/>
+      <c r="H4" s="100"/>
       <c r="J4" s="118"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5">
@@ -8157,11 +8125,11 @@
         <f>PEARSON($B$5:$B$56, $D$5:$D$56)</f>
         <v>-0.91720677499078029</v>
       </c>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="101"/>
-      <c r="N5" s="101"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="100"/>
       <c r="P5" s="95">
         <f>PEARSON($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.91720677499078029</v>
@@ -8171,7 +8139,7 @@
         <v>-0.91720677499078029</v>
       </c>
       <c r="R5">
-        <f>CORREL($B$5:$B$56, $D$5:$D$56)</f>
+        <f>CORREL($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.91720677499078029</v>
       </c>
     </row>
@@ -8203,11 +8171,11 @@
         <f>PEARSON($C$5:C$56, $E$5:E$56)</f>
         <v>-0.8811057107791842</v>
       </c>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100"/>
       <c r="P6" s="95">
         <f>PEARSON($E$5:E$56, $C$5:C$56)</f>
         <v>-0.8811057107791842</v>
@@ -8242,11 +8210,11 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="101"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8">
@@ -8272,11 +8240,11 @@
       <c r="G8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="101"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
+      <c r="N8" s="100"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9">
@@ -8306,11 +8274,11 @@
         <f>INTERCEPT($D$5:$D$56, $B$5:$B$56)</f>
         <v>46.129734040658491</v>
       </c>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="100"/>
+      <c r="M9" s="100"/>
+      <c r="N9" s="100"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10">
@@ -8340,11 +8308,11 @@
         <f>SLOPE($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.3967422303778369</v>
       </c>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="100"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11">
@@ -8374,11 +8342,11 @@
         <v>56</v>
       </c>
       <c r="I11" s="50"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="100"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="100"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12">
@@ -8408,11 +8376,11 @@
         <v>58</v>
       </c>
       <c r="I12" s="50"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="101"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="100"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="100"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1">
       <c r="A13" s="5">
@@ -8441,11 +8409,11 @@
         <f>D58*SQRT((1-H5^2)*((B59-1)/(B59-2)))</f>
         <v>3.6418560620845599</v>
       </c>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="101"/>
-      <c r="N13" s="101"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14">
@@ -8475,11 +8443,11 @@
         <f>H13/(B58*SQRT(B59-1))</f>
         <v>2.4599907197583686E-2</v>
       </c>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
+      <c r="J14" s="100"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
+      <c r="N14" s="100"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15">
@@ -8509,11 +8477,11 @@
         <f>H10/H14</f>
         <v>-16.127793783580074</v>
       </c>
-      <c r="J15" s="101"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="101"/>
-      <c r="M15" s="101"/>
-      <c r="N15" s="101"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="100"/>
+      <c r="L15" s="100"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1">
       <c r="A16">
@@ -8546,11 +8514,11 @@
       <c r="I16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="101"/>
-      <c r="N16" s="101"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="100"/>
+      <c r="L16" s="100"/>
+      <c r="M16" s="100"/>
+      <c r="N16" s="100"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17">
@@ -8792,7 +8760,7 @@
         <f>IF(ABS(H15)&gt;H20, "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="I24" s="101"/>
+      <c r="I24" s="100"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25">
@@ -8952,9 +8920,9 @@
       <c r="G29" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
-      <c r="J29" s="101"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="100"/>
       <c r="K29" s="64">
         <f>H9+H10*15</f>
         <v>40.178600584990939</v>
@@ -9040,7 +9008,7 @@
         <v>90</v>
       </c>
       <c r="H32" s="110"/>
-      <c r="I32" s="101"/>
+      <c r="I32" s="100"/>
       <c r="J32" s="111"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
@@ -9064,9 +9032,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="G33" s="101"/>
+      <c r="G33" s="100"/>
       <c r="H33" s="110"/>
-      <c r="I33" s="101"/>
+      <c r="I33" s="100"/>
       <c r="J33" s="111"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
@@ -9090,9 +9058,9 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="G34" s="101"/>
+      <c r="G34" s="100"/>
       <c r="H34" s="110"/>
-      <c r="I34" s="101"/>
+      <c r="I34" s="100"/>
       <c r="J34" s="111"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1">
@@ -9116,9 +9084,9 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="G35" s="101"/>
+      <c r="G35" s="100"/>
       <c r="H35" s="110"/>
-      <c r="I35" s="101"/>
+      <c r="I35" s="100"/>
       <c r="J35" s="111"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
@@ -9143,7 +9111,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="110"/>
-      <c r="I36" s="101"/>
+      <c r="I36" s="100"/>
       <c r="J36" s="111"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
@@ -9753,8 +9721,8 @@
       <c r="A1" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="45"/>
@@ -9896,10 +9864,10 @@
       <c r="D13" s="115" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
@@ -9940,7 +9908,7 @@
       <c r="F16" s="97"/>
       <c r="G16" s="97"/>
       <c r="H16" s="98"/>
-      <c r="I16" s="99" t="s">
+      <c r="I16" s="105" t="s">
         <v>112</v>
       </c>
       <c r="J16" s="98"/>
@@ -10050,7 +10018,7 @@
         <f>'Data Transformation'!C31+'Data Transformation'!F31-2</f>
         <v>50</v>
       </c>
-      <c r="C29" s="101"/>
+      <c r="C29" s="100"/>
       <c r="D29" s="5" t="s">
         <v>126</v>
       </c>
@@ -10063,7 +10031,7 @@
         <f>TINV(B19,B29)</f>
         <v>0.17204274843003223</v>
       </c>
-      <c r="C30" s="101"/>
+      <c r="C30" s="100"/>
       <c r="D30" s="5" t="s">
         <v>128</v>
       </c>
@@ -10076,7 +10044,7 @@
         <f>B23-'Data Transformation'!C42*B30</f>
         <v>2.9154700840650083E-3</v>
       </c>
-      <c r="C31" s="101"/>
+      <c r="C31" s="100"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15" t="s">
@@ -10086,7 +10054,7 @@
         <f>B23+'Data Transformation'!C42*B30</f>
         <v>1.997084529915935</v>
       </c>
-      <c r="C32" s="101"/>
+      <c r="C32" s="100"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="50"/>
@@ -10145,64 +10113,64 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="B39" s="110"/>
-      <c r="C39" s="101"/>
+      <c r="C39" s="100"/>
       <c r="D39" s="111"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="B40" s="110"/>
-      <c r="C40" s="101"/>
+      <c r="C40" s="100"/>
       <c r="D40" s="111"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="B41" s="110"/>
-      <c r="C41" s="101"/>
+      <c r="C41" s="100"/>
       <c r="D41" s="111"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="B42" s="110"/>
-      <c r="C42" s="101"/>
+      <c r="C42" s="100"/>
       <c r="D42" s="111"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="45"/>
       <c r="B43" s="110"/>
-      <c r="C43" s="101"/>
+      <c r="C43" s="100"/>
       <c r="D43" s="111"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
       <c r="A44" s="45"/>
       <c r="B44" s="110"/>
-      <c r="C44" s="101"/>
+      <c r="C44" s="100"/>
       <c r="D44" s="111"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
       <c r="A45" s="45"/>
       <c r="B45" s="110"/>
-      <c r="C45" s="101"/>
+      <c r="C45" s="100"/>
       <c r="D45" s="111"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
       <c r="A46" s="45"/>
       <c r="B46" s="110"/>
-      <c r="C46" s="101"/>
+      <c r="C46" s="100"/>
       <c r="D46" s="111"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
       <c r="A47" s="45"/>
       <c r="B47" s="110"/>
-      <c r="C47" s="101"/>
+      <c r="C47" s="100"/>
       <c r="D47" s="111"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
       <c r="A48" s="45"/>
       <c r="B48" s="110"/>
-      <c r="C48" s="101"/>
+      <c r="C48" s="100"/>
       <c r="D48" s="111"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="45"/>
       <c r="B49" s="110"/>
-      <c r="C49" s="101"/>
+      <c r="C49" s="100"/>
       <c r="D49" s="111"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Remove unnecessary unit_tests part in the notes inside A1_Solution
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DD8430-3295-974E-B1AB-7264A8A60046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CB20F3-A873-1D4A-A17C-D5F697964DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="15740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,18 +75,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">unit_tests:
-</t>
+          <t xml:space="preserve"> type: constant</t>
         </r>
       </text>
     </comment>
@@ -119,18 +108,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">unit_tests:
-</t>
+          <t xml:space="preserve"> type: constant</t>
         </r>
       </text>
     </comment>
@@ -163,18 +141,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">unit_tests:
-</t>
+          <t xml:space="preserve"> type: constant</t>
         </r>
       </text>
     </comment>
@@ -207,18 +174,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">unit_tests:
-</t>
+          <t xml:space="preserve"> type: constant</t>
         </r>
       </text>
     </comment>
@@ -251,18 +207,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">unit_tests:
-</t>
+          <t xml:space="preserve"> type: constant</t>
         </r>
       </text>
     </comment>
@@ -388,17 +333,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> - R5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">unit_tests:
-</t>
+          <t xml:space="preserve"> - R5</t>
         </r>
       </text>
     </comment>
@@ -469,25 +404,6 @@
           </rPr>
           <t xml:space="preserve"> - R6</t>
         </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>unit_tests:</t>
-        </r>
       </text>
     </comment>
     <comment ref="H9" authorId="0" shapeId="0" xr:uid="{A56C5C67-657A-1046-BDC4-1B0B65CD441E}">
@@ -519,17 +435,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: formula
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>unit_tests:</t>
+          <t xml:space="preserve"> type: formula</t>
         </r>
       </text>
     </comment>
@@ -562,18 +468,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: formula
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">unit_tests:
-</t>
+          <t xml:space="preserve"> type: formula</t>
         </r>
       </text>
     </comment>
@@ -606,17 +501,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>unit_tests:</t>
+          <t xml:space="preserve"> type: constant</t>
         </r>
       </text>
     </comment>
@@ -649,17 +534,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>unit_tests:</t>
+          <t xml:space="preserve"> type: constant</t>
         </r>
       </text>
     </comment>
@@ -6409,8 +6284,8 @@
   </sheetPr>
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="161" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46:I46"/>
+    <sheetView topLeftCell="A33" zoomScale="161" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7940,7 +7815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF0E198-CC32-F348-8C2B-88F5F685CD55}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -8006,8 +7881,8 @@
   </sheetPr>
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add use case for Delta checking in A1_Solution's relationships sheet
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/18980-GRA/pysheetgrader/sample_excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CB20F3-A873-1D4A-A17C-D5F697964DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49EE78B-7585-004F-8965-EC39A0146062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="15740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="9" r:id="rId1"/>
@@ -538,6 +538,49 @@
         </r>
       </text>
     </comment>
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{3857AB2B-00BF-8D44-AFCC-85CA7ADC7ADE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> delta: 0.001</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H21" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
@@ -744,7 +787,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="175">
   <si>
     <t>DO NOT MODIFY THE NEXT ROW</t>
   </si>
@@ -1268,6 +1311,9 @@
   </si>
   <si>
     <t>H6</t>
+  </si>
+  <si>
+    <t>H14</t>
   </si>
 </sst>
 </file>
@@ -1746,20 +1792,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2965,16 +3011,16 @@
     </row>
     <row r="2" spans="1:10" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101" t="s">
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
       <c r="I2" s="127" t="s">
         <v>135</v>
       </c>
@@ -3717,23 +3763,23 @@
         <v>4.0055133485154846</v>
       </c>
       <c r="H29" s="4"/>
-      <c r="I29" s="106"/>
-      <c r="J29" s="100"/>
-      <c r="K29" s="100"/>
-      <c r="L29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="101"/>
     </row>
     <row r="30" spans="1:12" ht="13">
       <c r="H30" s="4"/>
-      <c r="I30" s="106"/>
-      <c r="J30" s="100"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="100"/>
+      <c r="I30" s="100"/>
+      <c r="J30" s="101"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="101"/>
     </row>
     <row r="31" spans="1:12" ht="13">
       <c r="A31" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="100"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
@@ -3752,7 +3798,7 @@
       <c r="A32" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="100"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="2">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -3776,13 +3822,13 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="100"/>
+      <c r="L32" s="101"/>
     </row>
     <row r="33" spans="1:12" ht="13">
       <c r="A33" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="100"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="32">
         <f t="shared" ref="C33:D33" si="4">STDEVA(C$4:C$11, C$13:C$29)</f>
         <v>18.592928377925453</v>
@@ -3806,13 +3852,13 @@
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="100"/>
+      <c r="L33" s="101"/>
     </row>
     <row r="34" spans="1:12" ht="17.25" customHeight="1">
       <c r="A34" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="100"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="6">SKEW(C$4:C$11, C$13:C$29)</f>
         <v>0.24893711104029126</v>
@@ -3834,13 +3880,13 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="100"/>
+      <c r="L34" s="101"/>
     </row>
     <row r="35" spans="1:12" ht="13">
       <c r="A35" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="100"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="8">MEDIAN(C$4:C$11, C$13:C$29)</f>
         <v>57.68</v>
@@ -3864,13 +3910,13 @@
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="100"/>
+      <c r="L35" s="101"/>
     </row>
     <row r="36" spans="1:12" ht="13">
       <c r="A36" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="100"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="10">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -3895,13 +3941,13 @@
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="100"/>
+      <c r="L36" s="101"/>
     </row>
     <row r="37" spans="1:12" ht="13">
       <c r="A37" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="100"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="12">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -3923,7 +3969,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="100"/>
+      <c r="L37" s="101"/>
     </row>
     <row r="38" spans="1:12" ht="13">
       <c r="A38" s="15"/>
@@ -3936,7 +3982,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="100"/>
+      <c r="L38" s="101"/>
     </row>
     <row r="39" spans="1:12" ht="13">
       <c r="A39" s="15"/>
@@ -3954,13 +4000,13 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="100"/>
-    </row>
-    <row r="40" spans="1:12" ht="15">
+      <c r="L39" s="101"/>
+    </row>
+    <row r="40" spans="1:12" ht="14">
       <c r="A40" s="102" t="s">
         <v>138</v>
       </c>
-      <c r="B40" s="100"/>
+      <c r="B40" s="101"/>
       <c r="C40" s="51">
         <f>SQRT((C33^2*(C31-1)+F33^2*(F31-1))/(C31+F31-2))</f>
         <v>20.89619836575601</v>
@@ -3976,13 +4022,13 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="100"/>
-    </row>
-    <row r="41" spans="1:12" ht="15">
+      <c r="L40" s="101"/>
+    </row>
+    <row r="41" spans="1:12" ht="14">
       <c r="A41" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="100"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="32">
         <f t="shared" ref="C41:D41" si="14">ABS(C32-F32)</f>
         <v>1</v>
@@ -4001,7 +4047,7 @@
       <c r="A42" s="102" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="100"/>
+      <c r="B42" s="101"/>
       <c r="C42" s="32">
         <f t="shared" ref="C42:D42" si="15">SQRT(C33^2/$C31 + F33^2/$F31)</f>
         <v>5.7955626669230851</v>
@@ -4014,11 +4060,11 @@
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
     </row>
-    <row r="44" spans="1:12" ht="15">
+    <row r="44" spans="1:12" ht="14">
       <c r="A44" s="39"/>
       <c r="C44" s="93"/>
     </row>
-    <row r="45" spans="1:12" ht="15">
+    <row r="45" spans="1:12" ht="14">
       <c r="A45" s="15"/>
       <c r="C45" s="92"/>
     </row>
@@ -4031,6 +4077,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J22"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="L32:L40"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
@@ -4039,16 +4095,6 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="L32:L40"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J22"/>
-    <mergeCell ref="I29:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4119,7 +4165,7 @@
         <v>0.16000000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" ht="14">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4128,11 +4174,11 @@
       </c>
       <c r="C3" s="94">
         <f t="shared" ref="C3:C28" ca="1" si="0">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$3, $I$3)),0), 2)</f>
-        <v>44.25</v>
+        <v>49.36</v>
       </c>
       <c r="D3">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C5)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" s="33">
         <f>LN('Raw Data'!C5)</f>
@@ -4154,7 +4200,7 @@
         <v>606.97340451085847</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11" ht="14">
       <c r="A4" s="5">
         <f t="shared" ref="A4:A54" si="1">A3+1</f>
         <v>2</v>
@@ -4164,11 +4210,11 @@
       </c>
       <c r="C4" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>29.29</v>
+        <v>78.260000000000005</v>
       </c>
       <c r="D4">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C6)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="33">
         <f>LN('Raw Data'!C6)</f>
@@ -4179,7 +4225,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" ht="14">
       <c r="A5" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -4189,18 +4235,18 @@
       </c>
       <c r="C5" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>52.92</v>
+        <v>22.77</v>
       </c>
       <c r="D5">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C7)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" s="33">
         <f>LN('Raw Data'!C7)</f>
         <v>4.5709927341865049</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" ht="14">
       <c r="A6" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4210,11 +4256,11 @@
       </c>
       <c r="C6" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>65.75</v>
+        <v>47.26</v>
       </c>
       <c r="D6">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C8)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E6" s="33">
         <f>LN('Raw Data'!C8)</f>
@@ -4233,7 +4279,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" ht="14">
       <c r="A7" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -4243,7 +4289,7 @@
       </c>
       <c r="C7" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>48.31</v>
+        <v>47.32</v>
       </c>
       <c r="D7">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C9)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4267,7 +4313,7 @@
         <v>0.148225</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11" ht="14">
       <c r="A8" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4277,7 +4323,7 @@
       </c>
       <c r="C8" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>46.26</v>
+        <v>75.040000000000006</v>
       </c>
       <c r="D8">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C10)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4303,7 +4349,7 @@
         <v>610.46983794715493</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" ht="14">
       <c r="A9" s="5">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4313,7 +4359,7 @@
       </c>
       <c r="C9" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>74.94</v>
+        <v>53.54</v>
       </c>
       <c r="D9">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C11)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4328,7 +4374,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" ht="14">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -4338,11 +4384,11 @@
       </c>
       <c r="C10" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>11.48</v>
+        <v>79.45</v>
       </c>
       <c r="D10">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C12)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E10" s="33">
         <f>LN('Raw Data'!C12)</f>
@@ -4359,7 +4405,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11" ht="14">
       <c r="A11" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4369,11 +4415,11 @@
       </c>
       <c r="C11" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>23.97</v>
+        <v>77.69</v>
       </c>
       <c r="D11">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C13)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="33">
         <f>LN('Raw Data'!C13)</f>
@@ -4391,7 +4437,7 @@
       <c r="J11" s="21"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11" ht="14">
       <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4401,11 +4447,11 @@
       </c>
       <c r="C12" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>64.349999999999994</v>
+        <v>87.1</v>
       </c>
       <c r="D12">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C14)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E12" s="33">
         <f>LN('Raw Data'!C14)</f>
@@ -4419,7 +4465,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" ht="14">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -4429,11 +4475,11 @@
       </c>
       <c r="C13" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>82.71</v>
+        <v>52.36</v>
       </c>
       <c r="D13">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C15)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13" s="33">
         <f>LN('Raw Data'!C15)</f>
@@ -4447,7 +4493,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" ht="14">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -4457,18 +4503,18 @@
       </c>
       <c r="C14" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>16.440000000000001</v>
+        <v>43.01</v>
       </c>
       <c r="D14">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C16)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E14" s="33">
         <f>LN('Raw Data'!C16)</f>
         <v>4.1999050578825932</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" ht="14">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -4478,18 +4524,18 @@
       </c>
       <c r="C15" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>45.92</v>
       </c>
       <c r="D15">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C17)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E15" s="33">
         <f>LN('Raw Data'!C17)</f>
         <v>3.9304521408965134</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" ht="14">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4499,18 +4545,18 @@
       </c>
       <c r="C16" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>10.3</v>
       </c>
       <c r="D16">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C18)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E16" s="33">
         <f>LN('Raw Data'!C18)</f>
         <v>3.9485477801105184</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="14">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -4520,18 +4566,18 @@
       </c>
       <c r="C17" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>35.9</v>
+        <v>82.78</v>
       </c>
       <c r="D17">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C19)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E17" s="33">
         <f>LN('Raw Data'!C19)</f>
         <v>3.7357630400127868</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="14">
       <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -4541,18 +4587,18 @@
       </c>
       <c r="C18" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>58.08</v>
+        <v>36.64</v>
       </c>
       <c r="D18">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C20)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E18" s="33">
         <f>LN('Raw Data'!C20)</f>
         <v>2.6979998652487085</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="14">
       <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -4562,18 +4608,18 @@
       </c>
       <c r="C19" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>76.94</v>
+        <v>76.650000000000006</v>
       </c>
       <c r="D19">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C21)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E19" s="33">
         <f>LN('Raw Data'!C21)</f>
         <v>4.1277793383083381</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="14">
       <c r="A20" s="5">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -4583,18 +4629,18 @@
       </c>
       <c r="C20" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>53.35</v>
+        <v>100</v>
       </c>
       <c r="D20">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C22)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E20" s="33">
         <f>LN('Raw Data'!C22)</f>
         <v>3.8940626800511531</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="14">
       <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -4604,18 +4650,18 @@
       </c>
       <c r="C21" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>97.21</v>
+        <v>77.94</v>
       </c>
       <c r="D21">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C23)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="33">
         <f>LN('Raw Data'!C23)</f>
         <v>4.110217911378391</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5" ht="14">
       <c r="A22" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -4625,18 +4671,18 @@
       </c>
       <c r="C22" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>65.7</v>
+        <v>100</v>
       </c>
       <c r="D22">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C24)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E22" s="33">
         <f>LN('Raw Data'!C24)</f>
         <v>4.2158244597598102</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5" ht="14">
       <c r="A23" s="5">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -4646,18 +4692,18 @@
       </c>
       <c r="C23" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>70.319999999999993</v>
+        <v>79.739999999999995</v>
       </c>
       <c r="D23">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C25)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E23" s="33">
         <f>LN('Raw Data'!C25)</f>
         <v>4.0549104929766937</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:5" ht="14">
       <c r="A24" s="5">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -4667,18 +4713,18 @@
       </c>
       <c r="C24" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>61.78</v>
+        <v>65.91</v>
       </c>
       <c r="D24">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C26)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E24" s="33">
         <f>LN('Raw Data'!C26)</f>
         <v>4.2413267525707461</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:5" ht="14">
       <c r="A25" s="5">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -4688,18 +4734,18 @@
       </c>
       <c r="C25" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>38.020000000000003</v>
+        <v>78.02</v>
       </c>
       <c r="D25">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C27)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E25" s="33">
         <f>LN('Raw Data'!C27)</f>
         <v>4.0455043968026274</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15">
+    <row r="26" spans="1:5" ht="14">
       <c r="A26" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -4709,18 +4755,18 @@
       </c>
       <c r="C26" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>96.69</v>
+        <v>26.61</v>
       </c>
       <c r="D26">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C28)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E26" s="33">
         <f>LN('Raw Data'!C28)</f>
         <v>3.7106409458954492</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5" ht="14">
       <c r="A27" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -4730,18 +4776,18 @@
       </c>
       <c r="C27" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>25.47</v>
+        <v>38.03</v>
       </c>
       <c r="D27">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C29)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E27" s="33">
         <f>LN('Raw Data'!C29)</f>
         <v>3.9961803134348695</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15">
+    <row r="28" spans="1:5" ht="14">
       <c r="A28" s="5">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -4751,18 +4797,18 @@
       </c>
       <c r="C28" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>94.5</v>
+        <v>91.12</v>
       </c>
       <c r="D28">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C30)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E28" s="33">
         <f>LN('Raw Data'!C30)</f>
         <v>4.1108738641733114</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15">
+    <row r="29" spans="1:5" ht="14">
       <c r="A29" s="5">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -4772,18 +4818,18 @@
       </c>
       <c r="C29" s="94">
         <f t="shared" ref="C29:C54" ca="1" si="2">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$8, $I$8)),0), 2)</f>
-        <v>77.41</v>
+        <v>73.709999999999994</v>
       </c>
       <c r="D29">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C31)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="33">
         <f>LN('Raw Data'!C31)</f>
         <v>4.5860892981752999</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15">
+    <row r="30" spans="1:5" ht="14">
       <c r="A30" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -4793,18 +4839,18 @@
       </c>
       <c r="C30" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>21.79</v>
+        <v>97.36</v>
       </c>
       <c r="D30">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C32)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E30" s="33">
         <f>LN('Raw Data'!C32)</f>
         <v>4.1437694455496237</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15">
+    <row r="31" spans="1:5" ht="14">
       <c r="A31" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -4814,18 +4860,18 @@
       </c>
       <c r="C31" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>90.58</v>
+        <v>94.36</v>
       </c>
       <c r="D31">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C33)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E31" s="33">
         <f>LN('Raw Data'!C33)</f>
         <v>4.1436108035250188</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:5" ht="14">
       <c r="A32" s="5">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -4835,18 +4881,18 @@
       </c>
       <c r="C32" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>16.239999999999998</v>
+        <v>23.55</v>
       </c>
       <c r="D32">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C34)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E32" s="33">
         <f>LN('Raw Data'!C34)</f>
         <v>4.438643235092778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15">
+    <row r="33" spans="1:5" ht="14">
       <c r="A33" s="5">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -4856,18 +4902,18 @@
       </c>
       <c r="C33" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>79.72</v>
+        <v>100</v>
       </c>
       <c r="D33">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C35)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E33" s="33">
         <f>LN('Raw Data'!C35)</f>
         <v>3.942358205224219</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15">
+    <row r="34" spans="1:5" ht="14">
       <c r="A34" s="5">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -4877,18 +4923,18 @@
       </c>
       <c r="C34" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>68.41</v>
+        <v>67.91</v>
       </c>
       <c r="D34">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C36)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E34" s="33">
         <f>LN('Raw Data'!C36)</f>
         <v>3.8486571298063263</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15">
+    <row r="35" spans="1:5" ht="14">
       <c r="A35" s="5">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -4898,18 +4944,18 @@
       </c>
       <c r="C35" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>94.4</v>
+        <v>63.21</v>
       </c>
       <c r="D35">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C37)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E35" s="33">
         <f>LN('Raw Data'!C37)</f>
         <v>3.9425522104629689</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15">
+    <row r="36" spans="1:5" ht="14">
       <c r="A36" s="5">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -4919,18 +4965,18 @@
       </c>
       <c r="C36" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>60.39</v>
+        <v>79.3</v>
       </c>
       <c r="D36">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C38)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" s="33">
         <f>LN('Raw Data'!C38)</f>
         <v>3.9502817175452365</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15">
+    <row r="37" spans="1:5" ht="14">
       <c r="A37" s="5">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -4940,18 +4986,18 @@
       </c>
       <c r="C37" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>59.87</v>
+        <v>44.12</v>
       </c>
       <c r="D37">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C39)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E37" s="33">
         <f>LN('Raw Data'!C39)</f>
         <v>4.1052845022604352</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15">
+    <row r="38" spans="1:5" ht="14">
       <c r="A38" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -4961,18 +5007,18 @@
       </c>
       <c r="C38" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>84.25</v>
+        <v>46.69</v>
       </c>
       <c r="D38">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C40)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E38" s="33">
         <f>LN('Raw Data'!C40)</f>
         <v>3.9932342608529692</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15">
+    <row r="39" spans="1:5" ht="14">
       <c r="A39" s="5">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -4982,18 +5028,18 @@
       </c>
       <c r="C39" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>25.42</v>
+        <v>3.51</v>
       </c>
       <c r="D39">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C41)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E39" s="33">
         <f>LN('Raw Data'!C41)</f>
         <v>4.3330989610504584</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15">
+    <row r="40" spans="1:5" ht="14">
       <c r="A40" s="5">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -5003,7 +5049,7 @@
       </c>
       <c r="C40" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>24.55</v>
       </c>
       <c r="D40">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C42)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -5014,7 +5060,7 @@
         <v>4.3899948043230586</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15">
+    <row r="41" spans="1:5" ht="14">
       <c r="A41" s="5">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -5024,7 +5070,7 @@
       </c>
       <c r="C41" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>71.09</v>
+        <v>42.05</v>
       </c>
       <c r="D41">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C43)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -5035,7 +5081,7 @@
         <v>4.5332444464165027</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15">
+    <row r="42" spans="1:5" ht="14">
       <c r="A42" s="5">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -5045,18 +5091,18 @@
       </c>
       <c r="C42" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>65.58</v>
+        <v>54.47</v>
       </c>
       <c r="D42">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C44)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E42" s="33">
         <f>LN('Raw Data'!C44)</f>
         <v>2.0386195471595809</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15">
+    <row r="43" spans="1:5" ht="14">
       <c r="A43" s="5">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -5066,18 +5112,18 @@
       </c>
       <c r="C43" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>94.62</v>
+        <v>75.58</v>
       </c>
       <c r="D43">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C45)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E43" s="33">
         <f>LN('Raw Data'!C45)</f>
         <v>3.2872818575322613</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15">
+    <row r="44" spans="1:5" ht="14">
       <c r="A44" s="5">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -5087,18 +5133,18 @@
       </c>
       <c r="C44" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>40.729999999999997</v>
+        <v>56.46</v>
       </c>
       <c r="D44">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C46)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E44" s="33">
         <f>LN('Raw Data'!C46)</f>
         <v>4.2756934238792645</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15">
+    <row r="45" spans="1:5" ht="14">
       <c r="A45" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -5108,18 +5154,18 @@
       </c>
       <c r="C45" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>37.75</v>
+        <v>49.82</v>
       </c>
       <c r="D45">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C47)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E45" s="33">
         <f>LN('Raw Data'!C47)</f>
         <v>3.7972853279577228</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15">
+    <row r="46" spans="1:5" ht="14">
       <c r="A46" s="5">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -5129,18 +5175,18 @@
       </c>
       <c r="C46" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>69.239999999999995</v>
+        <v>100</v>
       </c>
       <c r="D46">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C48)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E46" s="33">
         <f>LN('Raw Data'!C48)</f>
         <v>3.9442965659784419</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15">
+    <row r="47" spans="1:5" ht="14">
       <c r="A47" s="5">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -5150,18 +5196,18 @@
       </c>
       <c r="C47" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>20.61</v>
+        <v>35.090000000000003</v>
       </c>
       <c r="D47">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C49)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E47" s="33">
         <f>LN('Raw Data'!C49)</f>
         <v>4.3384665199215018</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15">
+    <row r="48" spans="1:5" ht="14">
       <c r="A48" s="5">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -5171,18 +5217,18 @@
       </c>
       <c r="C48" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>63.58</v>
+        <v>55.88</v>
       </c>
       <c r="D48">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C50)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E48" s="33">
         <f>LN('Raw Data'!C50)</f>
         <v>4.6051701859880918</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15">
+    <row r="49" spans="1:5" ht="14">
       <c r="A49" s="5">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -5192,18 +5238,18 @@
       </c>
       <c r="C49" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>88.46</v>
+        <v>56.09</v>
       </c>
       <c r="D49">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C51)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E49" s="33">
         <f>LN('Raw Data'!C51)</f>
         <v>3.8097687713893897</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15">
+    <row r="50" spans="1:5" ht="14">
       <c r="A50" s="5">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -5213,7 +5259,7 @@
       </c>
       <c r="C50" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>47.6</v>
+        <v>67.11</v>
       </c>
       <c r="D50">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C52)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -5224,7 +5270,7 @@
         <v>4.0562964945845703</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15">
+    <row r="51" spans="1:5" ht="14">
       <c r="A51" s="5">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -5234,18 +5280,18 @@
       </c>
       <c r="C51" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>64.510000000000005</v>
+        <v>56.02</v>
       </c>
       <c r="D51">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C53)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E51" s="33">
         <f>LN('Raw Data'!C53)</f>
         <v>4.5951198501345898</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15">
+    <row r="52" spans="1:5" ht="14">
       <c r="A52" s="5">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -5255,18 +5301,18 @@
       </c>
       <c r="C52" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>37.71</v>
+        <v>63.11</v>
       </c>
       <c r="D52">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C54)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E52" s="33">
         <f>LN('Raw Data'!C54)</f>
         <v>3.6498787167642037</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15">
+    <row r="53" spans="1:5" ht="14">
       <c r="A53" s="5">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -5276,18 +5322,18 @@
       </c>
       <c r="C53" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>79.36</v>
+        <v>57.11</v>
       </c>
       <c r="D53">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C55)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E53" s="33">
         <f>LN('Raw Data'!C55)</f>
         <v>3.6030491975087431</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15">
+    <row r="54" spans="1:5" ht="14">
       <c r="A54" s="5">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -5297,11 +5343,11 @@
       </c>
       <c r="C54" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>62.32</v>
+        <v>51.17</v>
       </c>
       <c r="D54">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C56)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E54" s="33">
         <f>LN('Raw Data'!C56)</f>
@@ -5341,7 +5387,7 @@
       </c>
       <c r="B59" s="33">
         <f ca="1">AVERAGEA($C$3:$C$28)</f>
-        <v>57.293461538461543</v>
+        <v>62.416153846153833</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -5350,7 +5396,7 @@
       </c>
       <c r="B60" s="33">
         <f ca="1">AVERAGEA($C$29:$C$54)</f>
-        <v>62.37076923076922</v>
+        <v>59.162692307692296</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -5359,7 +5405,7 @@
       </c>
       <c r="B61" s="33">
         <f ca="1">STDEVA($C$3:$C$28)</f>
-        <v>25.295303902868234</v>
+        <v>24.406550608707196</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13">
@@ -5368,7 +5414,7 @@
       </c>
       <c r="B62" s="33">
         <f ca="1">STDEVA($C$29:$C$54)</f>
-        <v>24.67708620126405</v>
+        <v>23.768948577115026</v>
       </c>
     </row>
   </sheetData>
@@ -5458,7 +5504,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10" ht="14">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -5476,7 +5522,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10" ht="14">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -5494,7 +5540,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" ht="14">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -5508,7 +5554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10" ht="14">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -5526,7 +5572,7 @@
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10" ht="14">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -5544,7 +5590,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10" ht="14">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -5562,7 +5608,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="21"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10" ht="14">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -5580,7 +5626,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="15">
+    <row r="12" spans="1:10" ht="14">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -5597,7 +5643,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10" ht="14">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -5615,7 +5661,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" ht="14">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -5631,7 +5677,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" ht="14">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -5647,7 +5693,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10" ht="14">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -5661,7 +5707,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" ht="14">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -5675,7 +5721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" ht="14">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -5689,7 +5735,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
+    <row r="19" spans="1:4" ht="14">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -5703,7 +5749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="14">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -5717,7 +5763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4" ht="14">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -5731,7 +5777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4" ht="14">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -5745,7 +5791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" ht="14">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -5759,7 +5805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4" ht="14">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -5773,7 +5819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4" ht="14">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -5787,7 +5833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15">
+    <row r="26" spans="1:4" ht="14">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -5801,7 +5847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
+    <row r="27" spans="1:4" ht="14">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -5815,7 +5861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4" ht="14">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -5829,7 +5875,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4" ht="14">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -5843,7 +5889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" ht="14">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -5857,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15">
+    <row r="31" spans="1:4" ht="14">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -5871,7 +5917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15">
+    <row r="32" spans="1:4" ht="14">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -5885,7 +5931,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15">
+    <row r="33" spans="1:4" ht="14">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -5899,7 +5945,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15">
+    <row r="34" spans="1:4" ht="14">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -5913,7 +5959,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15">
+    <row r="35" spans="1:4" ht="14">
       <c r="A35" s="5">
         <v>31</v>
       </c>
@@ -5927,7 +5973,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15">
+    <row r="36" spans="1:4" ht="14">
       <c r="A36" s="5">
         <v>32</v>
       </c>
@@ -5941,7 +5987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15">
+    <row r="37" spans="1:4" ht="14">
       <c r="A37" s="5">
         <v>33</v>
       </c>
@@ -5955,7 +6001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15">
+    <row r="38" spans="1:4" ht="14">
       <c r="A38" s="5">
         <v>34</v>
       </c>
@@ -5969,7 +6015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15">
+    <row r="39" spans="1:4" ht="14">
       <c r="A39" s="5">
         <v>35</v>
       </c>
@@ -5983,7 +6029,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15">
+    <row r="40" spans="1:4" ht="14">
       <c r="A40" s="5">
         <v>36</v>
       </c>
@@ -5997,7 +6043,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15">
+    <row r="41" spans="1:4" ht="14">
       <c r="A41" s="5">
         <v>37</v>
       </c>
@@ -6011,7 +6057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15">
+    <row r="42" spans="1:4" ht="14">
       <c r="A42" s="5">
         <v>38</v>
       </c>
@@ -6025,7 +6071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15">
+    <row r="43" spans="1:4" ht="14">
       <c r="A43" s="5">
         <v>39</v>
       </c>
@@ -6039,7 +6085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15">
+    <row r="44" spans="1:4" ht="14">
       <c r="A44" s="5">
         <v>40</v>
       </c>
@@ -6053,7 +6099,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15">
+    <row r="45" spans="1:4" ht="14">
       <c r="A45" s="5">
         <v>41</v>
       </c>
@@ -6067,7 +6113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15">
+    <row r="46" spans="1:4" ht="14">
       <c r="A46" s="5">
         <v>42</v>
       </c>
@@ -6081,7 +6127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15">
+    <row r="47" spans="1:4" ht="14">
       <c r="A47" s="5">
         <v>43</v>
       </c>
@@ -6095,7 +6141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15">
+    <row r="48" spans="1:4" ht="14">
       <c r="A48" s="5">
         <v>44</v>
       </c>
@@ -6109,7 +6155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15">
+    <row r="49" spans="1:4" ht="14">
       <c r="A49" s="5">
         <v>45</v>
       </c>
@@ -6123,7 +6169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15">
+    <row r="50" spans="1:4" ht="14">
       <c r="A50" s="5">
         <v>46</v>
       </c>
@@ -6137,7 +6183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15">
+    <row r="51" spans="1:4" ht="14">
       <c r="A51" s="5">
         <v>47</v>
       </c>
@@ -6151,7 +6197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15">
+    <row r="52" spans="1:4" ht="14">
       <c r="A52" s="5">
         <v>48</v>
       </c>
@@ -6165,7 +6211,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15">
+    <row r="53" spans="1:4" ht="14">
       <c r="A53" s="5">
         <v>49</v>
       </c>
@@ -6179,7 +6225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15">
+    <row r="54" spans="1:4" ht="14">
       <c r="A54" s="5">
         <v>50</v>
       </c>
@@ -6193,7 +6239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15">
+    <row r="55" spans="1:4" ht="14">
       <c r="A55" s="5">
         <v>51</v>
       </c>
@@ -6207,7 +6253,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15">
+    <row r="56" spans="1:4" ht="14">
       <c r="A56" s="5">
         <v>52</v>
       </c>
@@ -6316,16 +6362,16 @@
     </row>
     <row r="2" spans="1:8" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101" t="s">
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
     </row>
     <row r="3" spans="1:8" ht="13">
       <c r="A3" s="5"/>
@@ -7028,13 +7074,13 @@
       <c r="A31" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="100"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
       </c>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
       <c r="F31" s="30">
         <f>COUNT(F$4:F$29)</f>
         <v>26</v>
@@ -7047,7 +7093,7 @@
       <c r="A32" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="100"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="0">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -7073,7 +7119,7 @@
       <c r="A33" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="100"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="32">
         <f>STDEV(C$4:C$29)</f>
         <v>18.729963016925137</v>
@@ -7096,7 +7142,7 @@
       <c r="A34" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="100"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="3">SKEW(C$4:C$29)</f>
         <v>0.30912598517031509</v>
@@ -7119,7 +7165,7 @@
       <c r="A35" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="100"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="5">MEDIAN(C$4:C$29)</f>
         <v>57.41</v>
@@ -7142,7 +7188,7 @@
       <c r="A36" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="100"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="7">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -7165,7 +7211,7 @@
       <c r="A37" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="100"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="9">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -7188,7 +7234,7 @@
       <c r="A38" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="100"/>
+      <c r="B38" s="101"/>
       <c r="C38" s="34">
         <f t="shared" ref="C38:D38" si="11">QUARTILE(C$4:C$29, 1)</f>
         <v>51.019999999999996</v>
@@ -7211,7 +7257,7 @@
       <c r="A39" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="100"/>
+      <c r="B39" s="101"/>
       <c r="C39" s="34">
         <f t="shared" ref="C39:D39" si="13">QUARTILE(C$4:C$29, 3)</f>
         <v>69.0625</v>
@@ -7234,7 +7280,7 @@
       <c r="A40" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="100"/>
+      <c r="B40" s="101"/>
       <c r="C40" s="36">
         <f t="shared" ref="C40:D40" si="15">MAX(0, C38-1.5*(C39-C38))</f>
         <v>23.95624999999999</v>
@@ -7257,7 +7303,7 @@
       <c r="A41" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="100"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="36">
         <f>MIN(C39+1.5*(C39-C38), 100)</f>
         <v>96.126249999999999</v>
@@ -7283,10 +7329,10 @@
       <c r="C43" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="100"/>
-      <c r="E43" s="100"/>
-      <c r="F43" s="100"/>
-      <c r="G43" s="100"/>
+      <c r="D43" s="101"/>
+      <c r="E43" s="101"/>
+      <c r="F43" s="101"/>
+      <c r="G43" s="101"/>
     </row>
     <row r="44" spans="1:9" ht="13">
       <c r="A44" s="39" t="s">
@@ -7331,7 +7377,7 @@
       <c r="E46" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="105" t="s">
+      <c r="F46" s="99" t="s">
         <v>36</v>
       </c>
       <c r="G46" s="97"/>
@@ -7356,7 +7402,7 @@
       <c r="E47" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F47" s="105" t="s">
+      <c r="F47" s="99" t="s">
         <v>36</v>
       </c>
       <c r="G47" s="97"/>
@@ -7381,7 +7427,7 @@
       <c r="E48" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="105" t="s">
+      <c r="F48" s="99" t="s">
         <v>36</v>
       </c>
       <c r="G48" s="97"/>
@@ -7406,7 +7452,7 @@
       <c r="E49" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="105" t="s">
+      <c r="F49" s="99" t="s">
         <v>36</v>
       </c>
       <c r="G49" s="97"/>
@@ -7431,7 +7477,7 @@
       <c r="E50" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="105" t="s">
+      <c r="F50" s="99" t="s">
         <v>36</v>
       </c>
       <c r="G50" s="97"/>
@@ -7676,8 +7722,8 @@
       <c r="J85" s="41"/>
     </row>
     <row r="94" spans="9:12" ht="13">
-      <c r="I94" s="106"/>
-      <c r="J94" s="100"/>
+      <c r="I94" s="100"/>
+      <c r="J94" s="101"/>
     </row>
     <row r="95" spans="9:12" ht="13">
       <c r="I95" s="4"/>
@@ -7685,11 +7731,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C43:G43"/>
@@ -7702,11 +7748,11 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="I94:J94"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C29">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
@@ -7881,8 +7927,8 @@
   </sheetPr>
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:N3"/>
+    <sheetView topLeftCell="G1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7938,10 +7984,10 @@
       <c r="J3" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="45" t="str">
@@ -7965,12 +8011,12 @@
       <c r="G4" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="100"/>
+      <c r="H4" s="101"/>
       <c r="J4" s="118"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5">
@@ -8000,11 +8046,11 @@
         <f>PEARSON($B$5:$B$56, $D$5:$D$56)</f>
         <v>-0.91720677499078029</v>
       </c>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
       <c r="P5" s="95">
         <f>PEARSON($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.91720677499078029</v>
@@ -8046,11 +8092,11 @@
         <f>PEARSON($C$5:C$56, $E$5:E$56)</f>
         <v>-0.8811057107791842</v>
       </c>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="101"/>
+      <c r="N6" s="101"/>
       <c r="P6" s="95">
         <f>PEARSON($E$5:E$56, $C$5:C$56)</f>
         <v>-0.8811057107791842</v>
@@ -8085,11 +8131,11 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="101"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8">
@@ -8115,11 +8161,11 @@
       <c r="G8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="100"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9">
@@ -8149,11 +8195,11 @@
         <f>INTERCEPT($D$5:$D$56, $B$5:$B$56)</f>
         <v>46.129734040658491</v>
       </c>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="101"/>
+      <c r="N9" s="101"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10">
@@ -8183,11 +8229,11 @@
         <f>SLOPE($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.3967422303778369</v>
       </c>
-      <c r="J10" s="100"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="100"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="100"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="101"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+      <c r="N10" s="101"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11">
@@ -8217,11 +8263,11 @@
         <v>56</v>
       </c>
       <c r="I11" s="50"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
+      <c r="J11" s="101"/>
+      <c r="K11" s="101"/>
+      <c r="L11" s="101"/>
+      <c r="M11" s="101"/>
+      <c r="N11" s="101"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12">
@@ -8251,11 +8297,11 @@
         <v>58</v>
       </c>
       <c r="I12" s="50"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="100"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1">
       <c r="A13" s="5">
@@ -8284,11 +8330,11 @@
         <f>D58*SQRT((1-H5^2)*((B59-1)/(B59-2)))</f>
         <v>3.6418560620845599</v>
       </c>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="101"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="101"/>
+      <c r="N13" s="101"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14">
@@ -8318,11 +8364,11 @@
         <f>H13/(B58*SQRT(B59-1))</f>
         <v>2.4599907197583686E-2</v>
       </c>
-      <c r="J14" s="100"/>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="100"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="101"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15">
@@ -8352,11 +8398,11 @@
         <f>H10/H14</f>
         <v>-16.127793783580074</v>
       </c>
-      <c r="J15" s="100"/>
-      <c r="K15" s="100"/>
-      <c r="L15" s="100"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="100"/>
+      <c r="J15" s="101"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="101"/>
+      <c r="M15" s="101"/>
+      <c r="N15" s="101"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1">
       <c r="A16">
@@ -8389,11 +8435,11 @@
       <c r="I16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="100"/>
-      <c r="K16" s="100"/>
-      <c r="L16" s="100"/>
-      <c r="M16" s="100"/>
-      <c r="N16" s="100"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+      <c r="N16" s="101"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17">
@@ -8635,7 +8681,7 @@
         <f>IF(ABS(H15)&gt;H20, "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="I24" s="100"/>
+      <c r="I24" s="101"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25">
@@ -8795,9 +8841,9 @@
       <c r="G29" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="100"/>
-      <c r="I29" s="100"/>
-      <c r="J29" s="100"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
       <c r="K29" s="64">
         <f>H9+H10*15</f>
         <v>40.178600584990939</v>
@@ -8883,7 +8929,7 @@
         <v>90</v>
       </c>
       <c r="H32" s="110"/>
-      <c r="I32" s="100"/>
+      <c r="I32" s="101"/>
       <c r="J32" s="111"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
@@ -8907,9 +8953,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="G33" s="100"/>
+      <c r="G33" s="101"/>
       <c r="H33" s="110"/>
-      <c r="I33" s="100"/>
+      <c r="I33" s="101"/>
       <c r="J33" s="111"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
@@ -8933,9 +8979,9 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="G34" s="100"/>
+      <c r="G34" s="101"/>
       <c r="H34" s="110"/>
-      <c r="I34" s="100"/>
+      <c r="I34" s="101"/>
       <c r="J34" s="111"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1">
@@ -8959,9 +9005,9 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="G35" s="100"/>
+      <c r="G35" s="101"/>
       <c r="H35" s="110"/>
-      <c r="I35" s="100"/>
+      <c r="I35" s="101"/>
       <c r="J35" s="111"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
@@ -8986,7 +9032,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="110"/>
-      <c r="I36" s="100"/>
+      <c r="I36" s="101"/>
       <c r="J36" s="111"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
@@ -9492,10 +9538,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA86947-E241-514A-AD1F-5C5A7FFCD94F}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9562,6 +9608,14 @@
       </c>
       <c r="B8" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -9596,8 +9650,8 @@
       <c r="A1" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="45"/>
@@ -9739,10 +9793,10 @@
       <c r="D13" s="115" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
@@ -9783,7 +9837,7 @@
       <c r="F16" s="97"/>
       <c r="G16" s="97"/>
       <c r="H16" s="98"/>
-      <c r="I16" s="105" t="s">
+      <c r="I16" s="99" t="s">
         <v>112</v>
       </c>
       <c r="J16" s="98"/>
@@ -9866,11 +9920,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5" ht="14">
       <c r="A27" s="45"/>
       <c r="E27" s="77"/>
     </row>
-    <row r="28" spans="1:5" ht="15">
+    <row r="28" spans="1:5" ht="14">
       <c r="A28" s="15" t="s">
         <v>123</v>
       </c>
@@ -9893,7 +9947,7 @@
         <f>'Data Transformation'!C31+'Data Transformation'!F31-2</f>
         <v>50</v>
       </c>
-      <c r="C29" s="100"/>
+      <c r="C29" s="101"/>
       <c r="D29" s="5" t="s">
         <v>126</v>
       </c>
@@ -9906,7 +9960,7 @@
         <f>TINV(B19,B29)</f>
         <v>0.17204274843003223</v>
       </c>
-      <c r="C30" s="100"/>
+      <c r="C30" s="101"/>
       <c r="D30" s="5" t="s">
         <v>128</v>
       </c>
@@ -9919,7 +9973,7 @@
         <f>B23-'Data Transformation'!C42*B30</f>
         <v>2.9154700840650083E-3</v>
       </c>
-      <c r="C31" s="100"/>
+      <c r="C31" s="101"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15" t="s">
@@ -9929,7 +9983,7 @@
         <f>B23+'Data Transformation'!C42*B30</f>
         <v>1.997084529915935</v>
       </c>
-      <c r="C32" s="100"/>
+      <c r="C32" s="101"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="50"/>
@@ -9988,64 +10042,64 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="B39" s="110"/>
-      <c r="C39" s="100"/>
+      <c r="C39" s="101"/>
       <c r="D39" s="111"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="B40" s="110"/>
-      <c r="C40" s="100"/>
+      <c r="C40" s="101"/>
       <c r="D40" s="111"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="B41" s="110"/>
-      <c r="C41" s="100"/>
+      <c r="C41" s="101"/>
       <c r="D41" s="111"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="B42" s="110"/>
-      <c r="C42" s="100"/>
+      <c r="C42" s="101"/>
       <c r="D42" s="111"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="45"/>
       <c r="B43" s="110"/>
-      <c r="C43" s="100"/>
+      <c r="C43" s="101"/>
       <c r="D43" s="111"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
       <c r="A44" s="45"/>
       <c r="B44" s="110"/>
-      <c r="C44" s="100"/>
+      <c r="C44" s="101"/>
       <c r="D44" s="111"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
       <c r="A45" s="45"/>
       <c r="B45" s="110"/>
-      <c r="C45" s="100"/>
+      <c r="C45" s="101"/>
       <c r="D45" s="111"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
       <c r="A46" s="45"/>
       <c r="B46" s="110"/>
-      <c r="C46" s="100"/>
+      <c r="C46" s="101"/>
       <c r="D46" s="111"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
       <c r="A47" s="45"/>
       <c r="B47" s="110"/>
-      <c r="C47" s="100"/>
+      <c r="C47" s="101"/>
       <c r="D47" s="111"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
       <c r="A48" s="45"/>
       <c r="B48" s="110"/>
-      <c r="C48" s="100"/>
+      <c r="C48" s="101"/>
       <c r="D48" s="111"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="45"/>
       <c r="B49" s="110"/>
-      <c r="C49" s="100"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="111"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Add sample note in A1_Solution for test case
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49EE78B-7585-004F-8965-EC39A0146062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576A558B-7879-2C48-B534-0EB68C5BF2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="9" r:id="rId1"/>
@@ -538,6 +538,220 @@
         </r>
       </text>
     </comment>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{47032891-F459-A74E-AFE4-7A2B56F84382}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve"> type: test</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t>test_cases:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve"> - default_test_case:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">    output: 3.642</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">    input:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">     D58: 9.05</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">     H5: -0.917</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">     B59: 52
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">    delta: 0.001</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">    </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H14" authorId="0" shapeId="0" xr:uid="{3857AB2B-00BF-8D44-AFCC-85CA7ADC7ADE}">
       <text>
         <r>
@@ -1326,7 +1540,7 @@
     <numFmt numFmtId="166" formatCode="0.000000000"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1399,6 +1613,12 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
     </font>
   </fonts>
   <fills count="8">
@@ -6330,8 +6550,8 @@
   </sheetPr>
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="161" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView topLeftCell="A18" zoomScale="161" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7927,8 +8147,8 @@
   </sheetPr>
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -9540,7 +9760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA86947-E241-514A-AD1F-5C5A7FFCD94F}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update A1_Solution's unit test notes
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576A558B-7879-2C48-B534-0EB68C5BF2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596F00A9-B937-CA41-B5E6-469FEFDEF707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="9" r:id="rId1"/>
@@ -538,25 +538,16 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{47032891-F459-A74E-AFE4-7A2B56F84382}">
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{A6D9E7F1-C2D1-FD4E-8ACF-9BF5CF93B4E8}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t>rubric:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">rubric:
 </t>
         </r>
         <r>
@@ -564,18 +555,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> score: 1
 </t>
         </r>
         <r>
@@ -583,18 +565,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: test</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> type: test
 </t>
         </r>
         <r>
@@ -602,18 +575,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t>test_cases:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">test_cases:
 </t>
         </r>
         <r>
@@ -621,9 +585,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> - default_test_case:
+          <t xml:space="preserve"> default_test_case:
 </t>
         </r>
         <r>
@@ -631,18 +595,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">    output: 3.642</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">    output: 3.642
 </t>
         </r>
         <r>
@@ -650,18 +605,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">    input:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">    input:
 </t>
         </r>
         <r>
@@ -669,18 +615,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">     D58: 9.05</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">     D58: 9.05
 </t>
         </r>
         <r>
@@ -688,18 +625,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">     H5: -0.917</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">     H5: -0.917
 </t>
         </r>
         <r>
@@ -707,7 +635,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">     B59: 52
 </t>
@@ -717,37 +645,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">    delta: 0.001</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">    </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">    delta: 0.001
 </t>
         </r>
       </text>
@@ -1001,7 +901,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="176">
   <si>
     <t>DO NOT MODIFY THE NEXT ROW</t>
   </si>
@@ -1528,6 +1428,9 @@
   </si>
   <si>
     <t>H14</t>
+  </si>
+  <si>
+    <t>H13</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1443,7 @@
     <numFmt numFmtId="166" formatCode="0.000000000"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1613,12 +1516,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="34"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1816,7 +1713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2006,6 +1903,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3231,20 +3129,20 @@
     </row>
     <row r="2" spans="1:10" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="106" t="s">
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="I2" s="127" t="s">
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="I2" s="128" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="98"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="3" spans="1:10" ht="13">
       <c r="A3" s="5"/>
@@ -3266,8 +3164,8 @@
       <c r="G3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="128"/>
-      <c r="J3" s="109"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="110"/>
     </row>
     <row r="4" spans="1:10" ht="13">
       <c r="B4" s="55">
@@ -3294,8 +3192,8 @@
         <f t="shared" ref="G4:G29" si="1">LN(F4)</f>
         <v>4.5860892981752999</v>
       </c>
-      <c r="I4" s="110"/>
-      <c r="J4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="112"/>
     </row>
     <row r="5" spans="1:10" ht="13">
       <c r="B5" s="55">
@@ -3322,8 +3220,8 @@
         <f t="shared" si="1"/>
         <v>4.1437694455496237</v>
       </c>
-      <c r="I5" s="110"/>
-      <c r="J5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="112"/>
     </row>
     <row r="6" spans="1:10" ht="13">
       <c r="B6" s="55">
@@ -3350,8 +3248,8 @@
         <f t="shared" si="1"/>
         <v>4.1436108035250188</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="112"/>
     </row>
     <row r="7" spans="1:10" ht="13">
       <c r="B7" s="55">
@@ -3378,8 +3276,8 @@
         <f t="shared" si="1"/>
         <v>4.438643235092778</v>
       </c>
-      <c r="I7" s="110"/>
-      <c r="J7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="112"/>
     </row>
     <row r="8" spans="1:10" ht="13">
       <c r="B8" s="55">
@@ -3406,8 +3304,8 @@
         <f t="shared" si="1"/>
         <v>3.942358205224219</v>
       </c>
-      <c r="I8" s="110"/>
-      <c r="J8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="112"/>
     </row>
     <row r="9" spans="1:10" ht="13">
       <c r="B9" s="55">
@@ -3434,8 +3332,8 @@
         <f t="shared" si="1"/>
         <v>3.8486571298063263</v>
       </c>
-      <c r="I9" s="110"/>
-      <c r="J9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="112"/>
     </row>
     <row r="10" spans="1:10" ht="13">
       <c r="B10" s="55">
@@ -3462,8 +3360,8 @@
         <f t="shared" si="1"/>
         <v>3.9425522104629689</v>
       </c>
-      <c r="I10" s="110"/>
-      <c r="J10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="112"/>
     </row>
     <row r="11" spans="1:10" ht="13">
       <c r="B11" s="55">
@@ -3490,8 +3388,8 @@
         <f t="shared" si="1"/>
         <v>3.9502817175452365</v>
       </c>
-      <c r="I11" s="110"/>
-      <c r="J11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="112"/>
     </row>
     <row r="12" spans="1:10" ht="13">
       <c r="B12" s="55">
@@ -3518,8 +3416,8 @@
         <f t="shared" si="1"/>
         <v>4.1052845022604352</v>
       </c>
-      <c r="I12" s="110"/>
-      <c r="J12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="112"/>
     </row>
     <row r="13" spans="1:10" ht="13">
       <c r="B13" s="55">
@@ -3546,8 +3444,8 @@
         <f t="shared" si="1"/>
         <v>3.9932342608529692</v>
       </c>
-      <c r="I13" s="110"/>
-      <c r="J13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="112"/>
     </row>
     <row r="14" spans="1:10" ht="13">
       <c r="B14" s="55">
@@ -3574,8 +3472,8 @@
         <f t="shared" si="1"/>
         <v>4.3330989610504584</v>
       </c>
-      <c r="I14" s="110"/>
-      <c r="J14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="112"/>
     </row>
     <row r="15" spans="1:10" ht="13">
       <c r="B15" s="55">
@@ -3602,8 +3500,8 @@
         <f t="shared" si="1"/>
         <v>4.3899948043230586</v>
       </c>
-      <c r="I15" s="110"/>
-      <c r="J15" s="111"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="112"/>
     </row>
     <row r="16" spans="1:10" ht="13">
       <c r="B16" s="55">
@@ -3630,8 +3528,8 @@
         <f t="shared" si="1"/>
         <v>4.5332444464165027</v>
       </c>
-      <c r="I16" s="110"/>
-      <c r="J16" s="111"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="112"/>
     </row>
     <row r="17" spans="1:12" ht="13">
       <c r="B17" s="55">
@@ -3658,8 +3556,8 @@
         <f t="shared" si="1"/>
         <v>2.0386195471595809</v>
       </c>
-      <c r="I17" s="110"/>
-      <c r="J17" s="111"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="112"/>
     </row>
     <row r="18" spans="1:12" ht="13">
       <c r="B18" s="55">
@@ -3686,8 +3584,8 @@
         <f t="shared" si="1"/>
         <v>3.2872818575322613</v>
       </c>
-      <c r="I18" s="110"/>
-      <c r="J18" s="111"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="112"/>
     </row>
     <row r="19" spans="1:12" ht="13">
       <c r="B19" s="55">
@@ -3714,8 +3612,8 @@
         <f t="shared" si="1"/>
         <v>4.2756934238792645</v>
       </c>
-      <c r="I19" s="110"/>
-      <c r="J19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="112"/>
     </row>
     <row r="20" spans="1:12" ht="13">
       <c r="B20" s="55">
@@ -3742,8 +3640,8 @@
         <f t="shared" si="1"/>
         <v>3.7972853279577228</v>
       </c>
-      <c r="I20" s="110"/>
-      <c r="J20" s="111"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="112"/>
     </row>
     <row r="21" spans="1:12" ht="13">
       <c r="B21" s="55">
@@ -3770,8 +3668,8 @@
         <f t="shared" si="1"/>
         <v>3.9442965659784419</v>
       </c>
-      <c r="I21" s="110"/>
-      <c r="J21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="112"/>
     </row>
     <row r="22" spans="1:12" ht="13">
       <c r="B22" s="55">
@@ -3798,8 +3696,8 @@
         <f t="shared" si="1"/>
         <v>4.3384665199215018</v>
       </c>
-      <c r="I22" s="112"/>
-      <c r="J22" s="114"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="115"/>
     </row>
     <row r="23" spans="1:12" ht="13">
       <c r="B23" s="55">
@@ -3983,23 +3881,23 @@
         <v>4.0055133485154846</v>
       </c>
       <c r="H29" s="4"/>
-      <c r="I29" s="100"/>
-      <c r="J29" s="101"/>
-      <c r="K29" s="101"/>
-      <c r="L29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="102"/>
+      <c r="L29" s="102"/>
     </row>
     <row r="30" spans="1:12" ht="13">
       <c r="H30" s="4"/>
-      <c r="I30" s="100"/>
-      <c r="J30" s="101"/>
-      <c r="K30" s="100"/>
-      <c r="L30" s="101"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="102"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="102"/>
     </row>
     <row r="31" spans="1:12" ht="13">
-      <c r="A31" s="102" t="s">
+      <c r="A31" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="101"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
@@ -4015,10 +3913,10 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A32" s="102" t="s">
+      <c r="A32" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="101"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="2">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -4042,13 +3940,13 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="101"/>
+      <c r="L32" s="102"/>
     </row>
     <row r="33" spans="1:12" ht="13">
-      <c r="A33" s="102" t="s">
+      <c r="A33" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="101"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="32">
         <f t="shared" ref="C33:D33" si="4">STDEVA(C$4:C$11, C$13:C$29)</f>
         <v>18.592928377925453</v>
@@ -4072,13 +3970,13 @@
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="101"/>
+      <c r="L33" s="102"/>
     </row>
     <row r="34" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A34" s="102" t="s">
+      <c r="A34" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="101"/>
+      <c r="B34" s="102"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="6">SKEW(C$4:C$11, C$13:C$29)</f>
         <v>0.24893711104029126</v>
@@ -4100,13 +3998,13 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="101"/>
+      <c r="L34" s="102"/>
     </row>
     <row r="35" spans="1:12" ht="13">
-      <c r="A35" s="102" t="s">
+      <c r="A35" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="101"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="8">MEDIAN(C$4:C$11, C$13:C$29)</f>
         <v>57.68</v>
@@ -4130,13 +4028,13 @@
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="101"/>
+      <c r="L35" s="102"/>
     </row>
     <row r="36" spans="1:12" ht="13">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="101"/>
+      <c r="B36" s="102"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="10">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -4161,13 +4059,13 @@
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="101"/>
+      <c r="L36" s="102"/>
     </row>
     <row r="37" spans="1:12" ht="13">
-      <c r="A37" s="102" t="s">
+      <c r="A37" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="101"/>
+      <c r="B37" s="102"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="12">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -4189,7 +4087,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="101"/>
+      <c r="L37" s="102"/>
     </row>
     <row r="38" spans="1:12" ht="13">
       <c r="A38" s="15"/>
@@ -4202,7 +4100,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="101"/>
+      <c r="L38" s="102"/>
     </row>
     <row r="39" spans="1:12" ht="13">
       <c r="A39" s="15"/>
@@ -4220,13 +4118,13 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="101"/>
+      <c r="L39" s="102"/>
     </row>
     <row r="40" spans="1:12" ht="14">
-      <c r="A40" s="102" t="s">
+      <c r="A40" s="103" t="s">
         <v>138</v>
       </c>
-      <c r="B40" s="101"/>
+      <c r="B40" s="102"/>
       <c r="C40" s="51">
         <f>SQRT((C33^2*(C31-1)+F33^2*(F31-1))/(C31+F31-2))</f>
         <v>20.89619836575601</v>
@@ -4242,13 +4140,13 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="101"/>
+      <c r="L40" s="102"/>
     </row>
     <row r="41" spans="1:12" ht="14">
-      <c r="A41" s="102" t="s">
+      <c r="A41" s="103" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="101"/>
+      <c r="B41" s="102"/>
       <c r="C41" s="32">
         <f t="shared" ref="C41:D41" si="14">ABS(C32-F32)</f>
         <v>1</v>
@@ -4264,10 +4162,10 @@
       <c r="I41" s="92"/>
     </row>
     <row r="42" spans="1:12" ht="13">
-      <c r="A42" s="102" t="s">
+      <c r="A42" s="103" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="101"/>
+      <c r="B42" s="102"/>
       <c r="C42" s="32">
         <f t="shared" ref="C42:D42" si="15">SQRT(C33^2/$C31 + F33^2/$F31)</f>
         <v>5.7955626669230851</v>
@@ -4394,11 +4292,11 @@
       </c>
       <c r="C3" s="94">
         <f t="shared" ref="C3:C28" ca="1" si="0">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$3, $I$3)),0), 2)</f>
-        <v>49.36</v>
+        <v>61.2</v>
       </c>
       <c r="D3">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C5)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" s="33">
         <f>LN('Raw Data'!C5)</f>
@@ -4430,11 +4328,11 @@
       </c>
       <c r="C4" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>78.260000000000005</v>
+        <v>56.69</v>
       </c>
       <c r="D4">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C6)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E4" s="33">
         <f>LN('Raw Data'!C6)</f>
@@ -4455,11 +4353,11 @@
       </c>
       <c r="C5" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>22.77</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C7)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E5" s="33">
         <f>LN('Raw Data'!C7)</f>
@@ -4476,11 +4374,11 @@
       </c>
       <c r="C6" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>47.26</v>
+        <v>40.61</v>
       </c>
       <c r="D6">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C8)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E6" s="33">
         <f>LN('Raw Data'!C8)</f>
@@ -4509,11 +4407,11 @@
       </c>
       <c r="C7" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>47.32</v>
+        <v>45.99</v>
       </c>
       <c r="D7">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C9)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="33">
         <f>LN('Raw Data'!C9)</f>
@@ -4543,11 +4441,11 @@
       </c>
       <c r="C8" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>75.040000000000006</v>
+        <v>62.4</v>
       </c>
       <c r="D8">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C10)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E8" s="33">
         <f>LN('Raw Data'!C10)</f>
@@ -4579,11 +4477,11 @@
       </c>
       <c r="C9" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>53.54</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="D9">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C11)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E9" s="33">
         <f>LN('Raw Data'!C11)</f>
@@ -4604,11 +4502,11 @@
       </c>
       <c r="C10" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>79.45</v>
+        <v>84.35</v>
       </c>
       <c r="D10">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C12)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E10" s="33">
         <f>LN('Raw Data'!C12)</f>
@@ -4635,11 +4533,11 @@
       </c>
       <c r="C11" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>77.69</v>
+        <v>75.260000000000005</v>
       </c>
       <c r="D11">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C13)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="33">
         <f>LN('Raw Data'!C13)</f>
@@ -4667,11 +4565,11 @@
       </c>
       <c r="C12" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>87.1</v>
+        <v>56.03</v>
       </c>
       <c r="D12">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C14)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E12" s="33">
         <f>LN('Raw Data'!C14)</f>
@@ -4695,11 +4593,11 @@
       </c>
       <c r="C13" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>52.36</v>
+        <v>46.75</v>
       </c>
       <c r="D13">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C15)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E13" s="33">
         <f>LN('Raw Data'!C15)</f>
@@ -4723,11 +4621,11 @@
       </c>
       <c r="C14" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>43.01</v>
+        <v>13.47</v>
       </c>
       <c r="D14">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C16)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E14" s="33">
         <f>LN('Raw Data'!C16)</f>
@@ -4744,11 +4642,11 @@
       </c>
       <c r="C15" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>45.92</v>
+        <v>27.19</v>
       </c>
       <c r="D15">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C17)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E15" s="33">
         <f>LN('Raw Data'!C17)</f>
@@ -4765,11 +4663,11 @@
       </c>
       <c r="C16" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>10.3</v>
+        <v>100</v>
       </c>
       <c r="D16">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C18)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E16" s="33">
         <f>LN('Raw Data'!C18)</f>
@@ -4786,11 +4684,11 @@
       </c>
       <c r="C17" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>82.78</v>
+        <v>43.98</v>
       </c>
       <c r="D17">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C19)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E17" s="33">
         <f>LN('Raw Data'!C19)</f>
@@ -4807,11 +4705,11 @@
       </c>
       <c r="C18" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>36.64</v>
+        <v>99.99</v>
       </c>
       <c r="D18">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C20)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E18" s="33">
         <f>LN('Raw Data'!C20)</f>
@@ -4828,11 +4726,11 @@
       </c>
       <c r="C19" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>76.650000000000006</v>
+        <v>59.23</v>
       </c>
       <c r="D19">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C21)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E19" s="33">
         <f>LN('Raw Data'!C21)</f>
@@ -4849,11 +4747,11 @@
       </c>
       <c r="C20" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>5.78</v>
       </c>
       <c r="D20">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C22)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E20" s="33">
         <f>LN('Raw Data'!C22)</f>
@@ -4870,11 +4768,11 @@
       </c>
       <c r="C21" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>77.94</v>
+        <v>93.98</v>
       </c>
       <c r="D21">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C23)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E21" s="33">
         <f>LN('Raw Data'!C23)</f>
@@ -4891,11 +4789,11 @@
       </c>
       <c r="C22" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>38.229999999999997</v>
       </c>
       <c r="D22">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C24)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E22" s="33">
         <f>LN('Raw Data'!C24)</f>
@@ -4912,11 +4810,11 @@
       </c>
       <c r="C23" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>79.739999999999995</v>
+        <v>38.71</v>
       </c>
       <c r="D23">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C25)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E23" s="33">
         <f>LN('Raw Data'!C25)</f>
@@ -4933,7 +4831,7 @@
       </c>
       <c r="C24" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>65.91</v>
+        <v>96.75</v>
       </c>
       <c r="D24">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C26)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4954,11 +4852,11 @@
       </c>
       <c r="C25" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>78.02</v>
+        <v>47.54</v>
       </c>
       <c r="D25">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C27)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E25" s="33">
         <f>LN('Raw Data'!C27)</f>
@@ -4975,7 +4873,7 @@
       </c>
       <c r="C26" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>26.61</v>
+        <v>61.55</v>
       </c>
       <c r="D26">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C28)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4996,11 +4894,11 @@
       </c>
       <c r="C27" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>38.03</v>
+        <v>49.38</v>
       </c>
       <c r="D27">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C29)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E27" s="33">
         <f>LN('Raw Data'!C29)</f>
@@ -5017,11 +4915,11 @@
       </c>
       <c r="C28" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>91.12</v>
+        <v>63.59</v>
       </c>
       <c r="D28">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C30)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E28" s="33">
         <f>LN('Raw Data'!C30)</f>
@@ -5038,11 +4936,11 @@
       </c>
       <c r="C29" s="94">
         <f t="shared" ref="C29:C54" ca="1" si="2">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$8, $I$8)),0), 2)</f>
-        <v>73.709999999999994</v>
+        <v>77.78</v>
       </c>
       <c r="D29">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C31)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E29" s="33">
         <f>LN('Raw Data'!C31)</f>
@@ -5059,7 +4957,7 @@
       </c>
       <c r="C30" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>97.36</v>
+        <v>84.85</v>
       </c>
       <c r="D30">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C32)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -5080,11 +4978,11 @@
       </c>
       <c r="C31" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>94.36</v>
+        <v>35.07</v>
       </c>
       <c r="D31">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C33)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E31" s="33">
         <f>LN('Raw Data'!C33)</f>
@@ -5101,11 +4999,11 @@
       </c>
       <c r="C32" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>23.55</v>
+        <v>59.71</v>
       </c>
       <c r="D32">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C34)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E32" s="33">
         <f>LN('Raw Data'!C34)</f>
@@ -5122,11 +5020,11 @@
       </c>
       <c r="C33" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>62.36</v>
       </c>
       <c r="D33">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C35)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E33" s="33">
         <f>LN('Raw Data'!C35)</f>
@@ -5143,11 +5041,11 @@
       </c>
       <c r="C34" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>67.91</v>
+        <v>81.83</v>
       </c>
       <c r="D34">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C36)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E34" s="33">
         <f>LN('Raw Data'!C36)</f>
@@ -5164,11 +5062,11 @@
       </c>
       <c r="C35" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>63.21</v>
+        <v>34.1</v>
       </c>
       <c r="D35">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C37)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E35" s="33">
         <f>LN('Raw Data'!C37)</f>
@@ -5185,11 +5083,11 @@
       </c>
       <c r="C36" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>79.3</v>
+        <v>50.63</v>
       </c>
       <c r="D36">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C38)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E36" s="33">
         <f>LN('Raw Data'!C38)</f>
@@ -5206,11 +5104,11 @@
       </c>
       <c r="C37" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>44.12</v>
+        <v>69.14</v>
       </c>
       <c r="D37">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C39)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E37" s="33">
         <f>LN('Raw Data'!C39)</f>
@@ -5227,11 +5125,11 @@
       </c>
       <c r="C38" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>46.69</v>
+        <v>58.15</v>
       </c>
       <c r="D38">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C40)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E38" s="33">
         <f>LN('Raw Data'!C40)</f>
@@ -5248,11 +5146,11 @@
       </c>
       <c r="C39" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>3.51</v>
+        <v>71.55</v>
       </c>
       <c r="D39">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C41)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E39" s="33">
         <f>LN('Raw Data'!C41)</f>
@@ -5269,11 +5167,11 @@
       </c>
       <c r="C40" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>24.55</v>
+        <v>84.18</v>
       </c>
       <c r="D40">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C42)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E40" s="33">
         <f>LN('Raw Data'!C42)</f>
@@ -5290,11 +5188,11 @@
       </c>
       <c r="C41" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>42.05</v>
+        <v>46.78</v>
       </c>
       <c r="D41">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C43)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E41" s="33">
         <f>LN('Raw Data'!C43)</f>
@@ -5311,11 +5209,11 @@
       </c>
       <c r="C42" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>54.47</v>
+        <v>60.32</v>
       </c>
       <c r="D42">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C44)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E42" s="33">
         <f>LN('Raw Data'!C44)</f>
@@ -5332,11 +5230,11 @@
       </c>
       <c r="C43" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>75.58</v>
+        <v>85.17</v>
       </c>
       <c r="D43">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C45)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E43" s="33">
         <f>LN('Raw Data'!C45)</f>
@@ -5353,11 +5251,11 @@
       </c>
       <c r="C44" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>56.46</v>
+        <v>29.63</v>
       </c>
       <c r="D44">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C46)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E44" s="33">
         <f>LN('Raw Data'!C46)</f>
@@ -5374,11 +5272,11 @@
       </c>
       <c r="C45" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>49.82</v>
+        <v>100</v>
       </c>
       <c r="D45">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C47)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E45" s="33">
         <f>LN('Raw Data'!C47)</f>
@@ -5395,11 +5293,11 @@
       </c>
       <c r="C46" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>21.4</v>
       </c>
       <c r="D46">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C48)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E46" s="33">
         <f>LN('Raw Data'!C48)</f>
@@ -5416,11 +5314,11 @@
       </c>
       <c r="C47" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>35.090000000000003</v>
+        <v>55.92</v>
       </c>
       <c r="D47">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C49)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E47" s="33">
         <f>LN('Raw Data'!C49)</f>
@@ -5437,11 +5335,11 @@
       </c>
       <c r="C48" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>55.88</v>
+        <v>55.08</v>
       </c>
       <c r="D48">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C50)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E48" s="33">
         <f>LN('Raw Data'!C50)</f>
@@ -5458,11 +5356,11 @@
       </c>
       <c r="C49" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>56.09</v>
+        <v>90.65</v>
       </c>
       <c r="D49">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C51)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E49" s="33">
         <f>LN('Raw Data'!C51)</f>
@@ -5479,11 +5377,11 @@
       </c>
       <c r="C50" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>67.11</v>
+        <v>65.23</v>
       </c>
       <c r="D50">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C52)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E50" s="33">
         <f>LN('Raw Data'!C52)</f>
@@ -5500,11 +5398,11 @@
       </c>
       <c r="C51" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>56.02</v>
+        <v>51.97</v>
       </c>
       <c r="D51">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C53)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E51" s="33">
         <f>LN('Raw Data'!C53)</f>
@@ -5521,11 +5419,11 @@
       </c>
       <c r="C52" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>63.11</v>
+        <v>26.13</v>
       </c>
       <c r="D52">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C54)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E52" s="33">
         <f>LN('Raw Data'!C54)</f>
@@ -5542,11 +5440,11 @@
       </c>
       <c r="C53" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>57.11</v>
+        <v>80.739999999999995</v>
       </c>
       <c r="D53">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C55)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E53" s="33">
         <f>LN('Raw Data'!C55)</f>
@@ -5563,11 +5461,11 @@
       </c>
       <c r="C54" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>51.17</v>
+        <v>73.53</v>
       </c>
       <c r="D54">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C56)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E54" s="33">
         <f>LN('Raw Data'!C56)</f>
@@ -5607,7 +5505,7 @@
       </c>
       <c r="B59" s="33">
         <f ca="1">AVERAGEA($C$3:$C$28)</f>
-        <v>62.416153846153833</v>
+        <v>54.061538461538461</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -5616,7 +5514,7 @@
       </c>
       <c r="B60" s="33">
         <f ca="1">AVERAGEA($C$29:$C$54)</f>
-        <v>59.162692307692296</v>
+        <v>61.996153846153859</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -5625,7 +5523,7 @@
       </c>
       <c r="B61" s="33">
         <f ca="1">STDEVA($C$3:$C$28)</f>
-        <v>24.406550608707196</v>
+        <v>26.963257324337906</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13">
@@ -5634,7 +5532,7 @@
       </c>
       <c r="B62" s="33">
         <f ca="1">STDEVA($C$29:$C$54)</f>
-        <v>23.768948577115026</v>
+        <v>21.119273676321917</v>
       </c>
     </row>
   </sheetData>
@@ -6491,34 +6389,34 @@
       <c r="A58" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="96">
+      <c r="B58" s="97">
         <f>COUNTIF($B$5:$B$56, "Solo")</f>
         <v>26</v>
       </c>
-      <c r="C58" s="97"/>
-      <c r="D58" s="98"/>
+      <c r="C58" s="98"/>
+      <c r="D58" s="99"/>
     </row>
     <row r="59" spans="1:4" ht="13">
       <c r="A59" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="96">
+      <c r="B59" s="97">
         <f>COUNTIF($B$5:$B$56, "Pair")</f>
         <v>26</v>
       </c>
-      <c r="C59" s="97"/>
-      <c r="D59" s="98"/>
+      <c r="C59" s="98"/>
+      <c r="D59" s="99"/>
     </row>
     <row r="60" spans="1:4" ht="13">
       <c r="A60" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B60" s="96">
+      <c r="B60" s="97">
         <f>B58+2*B59</f>
         <v>78</v>
       </c>
-      <c r="C60" s="97"/>
-      <c r="D60" s="98"/>
+      <c r="C60" s="98"/>
+      <c r="D60" s="99"/>
     </row>
     <row r="98" spans="12:13" ht="13">
       <c r="L98" s="27" t="s">
@@ -6582,16 +6480,16 @@
     </row>
     <row r="2" spans="1:8" ht="13">
       <c r="A2" s="4"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="106" t="s">
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
     </row>
     <row r="3" spans="1:8" ht="13">
       <c r="A3" s="5"/>
@@ -7291,16 +7189,16 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="13">
-      <c r="A31" s="102" t="s">
+      <c r="A31" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="101"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="30">
         <f>COUNT(C$4:C$29)</f>
         <v>26</v>
       </c>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
       <c r="F31" s="30">
         <f>COUNT(F$4:F$29)</f>
         <v>26</v>
@@ -7310,10 +7208,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A32" s="102" t="s">
+      <c r="A32" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="101"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="32">
         <f t="shared" ref="C32:D32" si="0">AVERAGE(C$4:C$29)</f>
         <v>60.02884615384616</v>
@@ -7336,10 +7234,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="13">
-      <c r="A33" s="102" t="s">
+      <c r="A33" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="101"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="32">
         <f>STDEV(C$4:C$29)</f>
         <v>18.729963016925137</v>
@@ -7359,10 +7257,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A34" s="102" t="s">
+      <c r="A34" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="101"/>
+      <c r="B34" s="102"/>
       <c r="C34" s="32">
         <f t="shared" ref="C34:D34" si="3">SKEW(C$4:C$29)</f>
         <v>0.30912598517031509</v>
@@ -7382,10 +7280,10 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="13">
-      <c r="A35" s="102" t="s">
+      <c r="A35" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="101"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="34">
         <f t="shared" ref="C35:D35" si="5">MEDIAN(C$4:C$29)</f>
         <v>57.41</v>
@@ -7405,10 +7303,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="13">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="101"/>
+      <c r="B36" s="102"/>
       <c r="C36" s="34">
         <f t="shared" ref="C36:D36" si="7">MIN(C$4:C$29)</f>
         <v>14.85</v>
@@ -7428,10 +7326,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="13">
-      <c r="A37" s="102" t="s">
+      <c r="A37" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="101"/>
+      <c r="B37" s="102"/>
       <c r="C37" s="34">
         <f t="shared" ref="C37:D37" si="9">MAX(C$4:C$29)</f>
         <v>100</v>
@@ -7451,10 +7349,10 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="13">
-      <c r="A38" s="102" t="s">
+      <c r="A38" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="34">
         <f t="shared" ref="C38:D38" si="11">QUARTILE(C$4:C$29, 1)</f>
         <v>51.019999999999996</v>
@@ -7474,10 +7372,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="13">
-      <c r="A39" s="102" t="s">
+      <c r="A39" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="101"/>
+      <c r="B39" s="102"/>
       <c r="C39" s="34">
         <f t="shared" ref="C39:D39" si="13">QUARTILE(C$4:C$29, 3)</f>
         <v>69.0625</v>
@@ -7497,10 +7395,10 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="13">
-      <c r="A40" s="102" t="s">
+      <c r="A40" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="101"/>
+      <c r="B40" s="102"/>
       <c r="C40" s="36">
         <f t="shared" ref="C40:D40" si="15">MAX(0, C38-1.5*(C39-C38))</f>
         <v>23.95624999999999</v>
@@ -7520,10 +7418,10 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="13">
-      <c r="A41" s="102" t="s">
+      <c r="A41" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="101"/>
+      <c r="B41" s="102"/>
       <c r="C41" s="36">
         <f>MIN(C39+1.5*(C39-C38), 100)</f>
         <v>96.126249999999999</v>
@@ -7546,13 +7444,13 @@
       <c r="A43" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="103" t="s">
+      <c r="C43" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="101"/>
-      <c r="E43" s="101"/>
-      <c r="F43" s="101"/>
-      <c r="G43" s="101"/>
+      <c r="D43" s="102"/>
+      <c r="E43" s="102"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="102"/>
     </row>
     <row r="44" spans="1:9" ht="13">
       <c r="A44" s="39" t="s">
@@ -7572,12 +7470,12 @@
       <c r="E45" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="104" t="s">
+      <c r="F45" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="G45" s="97"/>
-      <c r="H45" s="97"/>
-      <c r="I45" s="98"/>
+      <c r="G45" s="98"/>
+      <c r="H45" s="98"/>
+      <c r="I45" s="99"/>
     </row>
     <row r="46" spans="1:9" ht="13">
       <c r="A46" s="15" t="s">
@@ -7597,12 +7495,12 @@
       <c r="E46" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="99" t="s">
+      <c r="F46" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="97"/>
-      <c r="H46" s="97"/>
-      <c r="I46" s="98"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="98"/>
+      <c r="I46" s="99"/>
     </row>
     <row r="47" spans="1:9" ht="13">
       <c r="A47" s="15" t="s">
@@ -7622,12 +7520,12 @@
       <c r="E47" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F47" s="99" t="s">
+      <c r="F47" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="97"/>
-      <c r="H47" s="97"/>
-      <c r="I47" s="98"/>
+      <c r="G47" s="98"/>
+      <c r="H47" s="98"/>
+      <c r="I47" s="99"/>
     </row>
     <row r="48" spans="1:9" ht="13">
       <c r="A48" s="15" t="s">
@@ -7647,12 +7545,12 @@
       <c r="E48" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="99" t="s">
+      <c r="F48" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="G48" s="97"/>
-      <c r="H48" s="97"/>
-      <c r="I48" s="98"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="98"/>
+      <c r="I48" s="99"/>
     </row>
     <row r="49" spans="1:12" ht="13">
       <c r="A49" s="15" t="s">
@@ -7672,12 +7570,12 @@
       <c r="E49" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="99" t="s">
+      <c r="F49" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="G49" s="97"/>
-      <c r="H49" s="97"/>
-      <c r="I49" s="98"/>
+      <c r="G49" s="98"/>
+      <c r="H49" s="98"/>
+      <c r="I49" s="99"/>
     </row>
     <row r="50" spans="1:12" ht="13">
       <c r="A50" s="15" t="s">
@@ -7697,12 +7595,12 @@
       <c r="E50" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="99" t="s">
+      <c r="F50" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="G50" s="97"/>
-      <c r="H50" s="97"/>
-      <c r="I50" s="98"/>
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="99"/>
     </row>
     <row r="51" spans="1:12" ht="13">
       <c r="B51" s="5" t="s">
@@ -7942,8 +7840,8 @@
       <c r="J85" s="41"/>
     </row>
     <row r="94" spans="9:12" ht="13">
-      <c r="I94" s="100"/>
-      <c r="J94" s="101"/>
+      <c r="I94" s="101"/>
+      <c r="J94" s="102"/>
     </row>
     <row r="95" spans="9:12" ht="13">
       <c r="I95" s="4"/>
@@ -8147,7 +8045,7 @@
   </sheetPr>
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -8201,13 +8099,13 @@
       <c r="H3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="116" t="s">
+      <c r="J3" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="45" t="str">
@@ -8228,15 +8126,15 @@
       <c r="E4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="117" t="s">
+      <c r="G4" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="101"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
+      <c r="H4" s="102"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5">
@@ -8266,11 +8164,11 @@
         <f>PEARSON($B$5:$B$56, $D$5:$D$56)</f>
         <v>-0.91720677499078029</v>
       </c>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="101"/>
-      <c r="N5" s="101"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
       <c r="P5" s="95">
         <f>PEARSON($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.91720677499078029</v>
@@ -8312,11 +8210,11 @@
         <f>PEARSON($C$5:C$56, $E$5:E$56)</f>
         <v>-0.8811057107791842</v>
       </c>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
       <c r="P6" s="95">
         <f>PEARSON($E$5:E$56, $C$5:C$56)</f>
         <v>-0.8811057107791842</v>
@@ -8351,11 +8249,11 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="101"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8">
@@ -8381,11 +8279,11 @@
       <c r="G8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="101"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="102"/>
+      <c r="N8" s="102"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9">
@@ -8415,11 +8313,11 @@
         <f>INTERCEPT($D$5:$D$56, $B$5:$B$56)</f>
         <v>46.129734040658491</v>
       </c>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10">
@@ -8449,11 +8347,11 @@
         <f>SLOPE($D$5:$D$56, $B$5:$B$56)</f>
         <v>-0.3967422303778369</v>
       </c>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11">
@@ -8483,11 +8381,11 @@
         <v>56</v>
       </c>
       <c r="I11" s="50"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12">
@@ -8517,11 +8415,11 @@
         <v>58</v>
       </c>
       <c r="I12" s="50"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="101"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1">
       <c r="A13" s="5">
@@ -8550,11 +8448,11 @@
         <f>D58*SQRT((1-H5^2)*((B59-1)/(B59-2)))</f>
         <v>3.6418560620845599</v>
       </c>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="101"/>
-      <c r="N13" s="101"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14">
@@ -8584,11 +8482,11 @@
         <f>H13/(B58*SQRT(B59-1))</f>
         <v>2.4599907197583686E-2</v>
       </c>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15">
@@ -8618,11 +8516,11 @@
         <f>H10/H14</f>
         <v>-16.127793783580074</v>
       </c>
-      <c r="J15" s="101"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="101"/>
-      <c r="M15" s="101"/>
-      <c r="N15" s="101"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="102"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1">
       <c r="A16">
@@ -8655,11 +8553,11 @@
       <c r="I16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="101"/>
-      <c r="N16" s="101"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17">
@@ -8868,7 +8766,7 @@
         <f>IF(OR(0&lt;H21, 0&gt;H22), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="I23" s="119" t="s">
+      <c r="I23" s="120" t="s">
         <v>74</v>
       </c>
       <c r="J23" s="45"/>
@@ -8901,7 +8799,7 @@
         <f>IF(ABS(H15)&gt;H20, "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="I24" s="101"/>
+      <c r="I24" s="102"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25">
@@ -9058,12 +8956,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G29" s="102" t="s">
+      <c r="G29" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
-      <c r="J29" s="101"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
       <c r="K29" s="64">
         <f>H9+H10*15</f>
         <v>40.178600584990939</v>
@@ -9118,11 +9016,11 @@
       <c r="G31" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="H31" s="107" t="s">
+      <c r="H31" s="108" t="s">
         <v>89</v>
       </c>
-      <c r="I31" s="108"/>
-      <c r="J31" s="109"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="110"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1">
       <c r="A32">
@@ -9145,12 +9043,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="G32" s="115" t="s">
+      <c r="G32" s="116" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="110"/>
-      <c r="I32" s="101"/>
-      <c r="J32" s="111"/>
+      <c r="H32" s="111"/>
+      <c r="I32" s="102"/>
+      <c r="J32" s="112"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
       <c r="A33">
@@ -9173,10 +9071,10 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="G33" s="101"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="111"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="111"/>
+      <c r="I33" s="102"/>
+      <c r="J33" s="112"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34">
@@ -9199,10 +9097,10 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="G34" s="101"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="111"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="111"/>
+      <c r="I34" s="102"/>
+      <c r="J34" s="112"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1">
       <c r="A35">
@@ -9225,10 +9123,10 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="G35" s="101"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="101"/>
-      <c r="J35" s="111"/>
+      <c r="G35" s="102"/>
+      <c r="H35" s="111"/>
+      <c r="I35" s="102"/>
+      <c r="J35" s="112"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
       <c r="A36">
@@ -9251,9 +9149,9 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H36" s="110"/>
-      <c r="I36" s="101"/>
-      <c r="J36" s="111"/>
+      <c r="H36" s="111"/>
+      <c r="I36" s="102"/>
+      <c r="J36" s="112"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
       <c r="A37">
@@ -9276,9 +9174,9 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="H37" s="112"/>
-      <c r="I37" s="113"/>
-      <c r="J37" s="114"/>
+      <c r="H37" s="113"/>
+      <c r="I37" s="114"/>
+      <c r="J37" s="115"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38">
@@ -9758,10 +9656,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA86947-E241-514A-AD1F-5C5A7FFCD94F}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9835,11 +9733,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="96" t="s">
         <v>174</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9867,11 +9774,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="45"/>
@@ -9891,13 +9798,13 @@
       <c r="C4" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="122" t="s">
+      <c r="D4" s="123" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="99"/>
       <c r="I4" s="69"/>
       <c r="J4" s="69"/>
     </row>
@@ -9957,14 +9864,14 @@
       <c r="C8" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="122" t="str">
+      <c r="D8" s="123" t="str">
         <f>D4</f>
         <v>quality difference between solo and pair programmers.</v>
       </c>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="97"/>
-      <c r="H8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="99"/>
       <c r="I8" s="69"/>
       <c r="J8" s="69"/>
     </row>
@@ -10010,13 +9917,13 @@
       <c r="C13" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="115" t="s">
+      <c r="D13" s="116" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
@@ -10050,17 +9957,17 @@
       <c r="C16" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="123" t="s">
+      <c r="D16" s="124" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="99" t="s">
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="98"/>
+      <c r="J16" s="99"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="15"/>
@@ -10070,39 +9977,39 @@
       <c r="A18" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="120" t="s">
+      <c r="B18" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="98"/>
+      <c r="C18" s="99"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="124">
+      <c r="B19" s="125">
         <f>TTEST('Data Transformation'!C4:C29, 'Data Transformation'!F4:F29, 2, 2)</f>
         <v>0.86409838706386388</v>
       </c>
-      <c r="C19" s="98"/>
+      <c r="C19" s="99"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="104">
+      <c r="B20" s="105">
         <v>0.05</v>
       </c>
-      <c r="C20" s="98"/>
+      <c r="C20" s="99"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="120" t="s">
+      <c r="B21" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="98"/>
+      <c r="C21" s="99"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="45"/>
@@ -10152,7 +10059,7 @@
         <f>1-B19</f>
         <v>0.13590161293613612</v>
       </c>
-      <c r="C28" s="125" t="s">
+      <c r="C28" s="126" t="s">
         <v>124</v>
       </c>
       <c r="D28" s="79" t="s">
@@ -10167,7 +10074,7 @@
         <f>'Data Transformation'!C31+'Data Transformation'!F31-2</f>
         <v>50</v>
       </c>
-      <c r="C29" s="101"/>
+      <c r="C29" s="102"/>
       <c r="D29" s="5" t="s">
         <v>126</v>
       </c>
@@ -10180,7 +10087,7 @@
         <f>TINV(B19,B29)</f>
         <v>0.17204274843003223</v>
       </c>
-      <c r="C30" s="101"/>
+      <c r="C30" s="102"/>
       <c r="D30" s="5" t="s">
         <v>128</v>
       </c>
@@ -10193,7 +10100,7 @@
         <f>B23-'Data Transformation'!C42*B30</f>
         <v>2.9154700840650083E-3</v>
       </c>
-      <c r="C31" s="101"/>
+      <c r="C31" s="102"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15" t="s">
@@ -10203,7 +10110,7 @@
         <f>B23+'Data Transformation'!C42*B30</f>
         <v>1.997084529915935</v>
       </c>
-      <c r="C32" s="101"/>
+      <c r="C32" s="102"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="50"/>
@@ -10230,11 +10137,11 @@
       <c r="G35" s="67"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A36" s="126" t="s">
+      <c r="A36" s="127" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="113"/>
-      <c r="C36" s="113"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
       <c r="D36" s="83">
         <f>B31</f>
         <v>2.9154700840650083E-3</v>
@@ -10254,79 +10161,79 @@
       <c r="A38" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="121" t="s">
+      <c r="B38" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="108"/>
-      <c r="D38" s="109"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="110"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B39" s="110"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="111"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="102"/>
+      <c r="D39" s="112"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B40" s="110"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="111"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="112"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B41" s="110"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="111"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="102"/>
+      <c r="D41" s="112"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B42" s="110"/>
-      <c r="C42" s="101"/>
-      <c r="D42" s="111"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="102"/>
+      <c r="D42" s="112"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="45"/>
-      <c r="B43" s="110"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="111"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="102"/>
+      <c r="D43" s="112"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1">
       <c r="A44" s="45"/>
-      <c r="B44" s="110"/>
-      <c r="C44" s="101"/>
-      <c r="D44" s="111"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="102"/>
+      <c r="D44" s="112"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1">
       <c r="A45" s="45"/>
-      <c r="B45" s="110"/>
-      <c r="C45" s="101"/>
-      <c r="D45" s="111"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="102"/>
+      <c r="D45" s="112"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
       <c r="A46" s="45"/>
-      <c r="B46" s="110"/>
-      <c r="C46" s="101"/>
-      <c r="D46" s="111"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="102"/>
+      <c r="D46" s="112"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1">
       <c r="A47" s="45"/>
-      <c r="B47" s="110"/>
-      <c r="C47" s="101"/>
-      <c r="D47" s="111"/>
+      <c r="B47" s="111"/>
+      <c r="C47" s="102"/>
+      <c r="D47" s="112"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1">
       <c r="A48" s="45"/>
-      <c r="B48" s="110"/>
-      <c r="C48" s="101"/>
-      <c r="D48" s="111"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="102"/>
+      <c r="D48" s="112"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="45"/>
-      <c r="B49" s="110"/>
-      <c r="C49" s="101"/>
-      <c r="D49" s="111"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="102"/>
+      <c r="D49" s="112"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="45"/>
-      <c r="B50" s="112"/>
-      <c r="C50" s="113"/>
-      <c r="D50" s="114"/>
+      <c r="B50" s="113"/>
+      <c r="C50" s="114"/>
+      <c r="D50" s="115"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="45"/>

</xml_diff>

<commit_message>
Minor changes to A1_Solution
</commit_message>
<xml_diff>
--- a/sample_excel_files/A1_Solution.xlsx
+++ b/sample_excel_files/A1_Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596F00A9-B937-CA41-B5E6-469FEFDEF707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4AC2D3-0892-8A48-AF65-BDDD773C355D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="19300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="9" r:id="rId1"/>
@@ -4292,11 +4292,11 @@
       </c>
       <c r="C3" s="94">
         <f t="shared" ref="C3:C28" ca="1" si="0">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$3, $I$3)),0), 2)</f>
-        <v>61.2</v>
+        <v>27.44</v>
       </c>
       <c r="D3">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C5)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" s="33">
         <f>LN('Raw Data'!C5)</f>
@@ -4328,11 +4328,11 @@
       </c>
       <c r="C4" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>56.69</v>
+        <v>69.67</v>
       </c>
       <c r="D4">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C6)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" s="33">
         <f>LN('Raw Data'!C6)</f>
@@ -4353,11 +4353,11 @@
       </c>
       <c r="C5" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>59.24</v>
       </c>
       <c r="D5">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C7)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E5" s="33">
         <f>LN('Raw Data'!C7)</f>
@@ -4374,11 +4374,11 @@
       </c>
       <c r="C6" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>40.61</v>
+        <v>86.73</v>
       </c>
       <c r="D6">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C8)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E6" s="33">
         <f>LN('Raw Data'!C8)</f>
@@ -4407,11 +4407,11 @@
       </c>
       <c r="C7" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>45.99</v>
+        <v>66.67</v>
       </c>
       <c r="D7">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C9)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E7" s="33">
         <f>LN('Raw Data'!C9)</f>
@@ -4441,11 +4441,11 @@
       </c>
       <c r="C8" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>62.4</v>
+        <v>40.29</v>
       </c>
       <c r="D8">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C10)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E8" s="33">
         <f>LN('Raw Data'!C10)</f>
@@ -4477,11 +4477,11 @@
       </c>
       <c r="C9" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>36.950000000000003</v>
+        <v>64.31</v>
       </c>
       <c r="D9">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C11)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E9" s="33">
         <f>LN('Raw Data'!C11)</f>
@@ -4502,11 +4502,11 @@
       </c>
       <c r="C10" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>84.35</v>
+        <v>50.99</v>
       </c>
       <c r="D10">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C12)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" s="33">
         <f>LN('Raw Data'!C12)</f>
@@ -4533,11 +4533,11 @@
       </c>
       <c r="C11" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>75.260000000000005</v>
+        <v>47.32</v>
       </c>
       <c r="D11">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C13)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="33">
         <f>LN('Raw Data'!C13)</f>
@@ -4565,11 +4565,11 @@
       </c>
       <c r="C12" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>56.03</v>
+        <v>93.77</v>
       </c>
       <c r="D12">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C14)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E12" s="33">
         <f>LN('Raw Data'!C14)</f>
@@ -4593,11 +4593,11 @@
       </c>
       <c r="C13" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>46.75</v>
+        <v>38.549999999999997</v>
       </c>
       <c r="D13">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C15)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E13" s="33">
         <f>LN('Raw Data'!C15)</f>
@@ -4621,11 +4621,11 @@
       </c>
       <c r="C14" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>13.47</v>
+        <v>67.739999999999995</v>
       </c>
       <c r="D14">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C16)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="33">
         <f>LN('Raw Data'!C16)</f>
@@ -4642,11 +4642,11 @@
       </c>
       <c r="C15" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>27.19</v>
+        <v>63.24</v>
       </c>
       <c r="D15">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C17)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="33">
         <f>LN('Raw Data'!C17)</f>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="D16">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C18)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E16" s="33">
         <f>LN('Raw Data'!C18)</f>
@@ -4684,11 +4684,11 @@
       </c>
       <c r="C17" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>43.98</v>
+        <v>46.54</v>
       </c>
       <c r="D17">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C19)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E17" s="33">
         <f>LN('Raw Data'!C19)</f>
@@ -4705,11 +4705,11 @@
       </c>
       <c r="C18" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>99.99</v>
+        <v>47.24</v>
       </c>
       <c r="D18">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C20)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="33">
         <f>LN('Raw Data'!C20)</f>
@@ -4726,11 +4726,11 @@
       </c>
       <c r="C19" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>59.23</v>
+        <v>35.590000000000003</v>
       </c>
       <c r="D19">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C21)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E19" s="33">
         <f>LN('Raw Data'!C21)</f>
@@ -4747,11 +4747,11 @@
       </c>
       <c r="C20" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>5.78</v>
+        <v>53.3</v>
       </c>
       <c r="D20">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C22)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E20" s="33">
         <f>LN('Raw Data'!C22)</f>
@@ -4768,11 +4768,11 @@
       </c>
       <c r="C21" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>93.98</v>
+        <v>47.84</v>
       </c>
       <c r="D21">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C23)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E21" s="33">
         <f>LN('Raw Data'!C23)</f>
@@ -4789,11 +4789,11 @@
       </c>
       <c r="C22" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>38.229999999999997</v>
+        <v>100</v>
       </c>
       <c r="D22">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C24)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22" s="33">
         <f>LN('Raw Data'!C24)</f>
@@ -4810,11 +4810,11 @@
       </c>
       <c r="C23" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>38.71</v>
+        <v>66.14</v>
       </c>
       <c r="D23">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C25)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E23" s="33">
         <f>LN('Raw Data'!C25)</f>
@@ -4831,11 +4831,11 @@
       </c>
       <c r="C24" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>96.75</v>
+        <v>7.1</v>
       </c>
       <c r="D24">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C26)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E24" s="33">
         <f>LN('Raw Data'!C26)</f>
@@ -4852,7 +4852,7 @@
       </c>
       <c r="C25" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>47.54</v>
+        <v>69.39</v>
       </c>
       <c r="D25">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C27)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4873,11 +4873,11 @@
       </c>
       <c r="C26" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>61.55</v>
+        <v>67.989999999999995</v>
       </c>
       <c r="D26">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C28)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E26" s="33">
         <f>LN('Raw Data'!C28)</f>
@@ -4894,11 +4894,11 @@
       </c>
       <c r="C27" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>49.38</v>
+        <v>26.32</v>
       </c>
       <c r="D27">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C29)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E27" s="33">
         <f>LN('Raw Data'!C29)</f>
@@ -4915,11 +4915,11 @@
       </c>
       <c r="C28" s="94">
         <f t="shared" ca="1" si="0"/>
-        <v>63.59</v>
+        <v>48.49</v>
       </c>
       <c r="D28">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C30)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E28" s="33">
         <f>LN('Raw Data'!C30)</f>
@@ -4936,11 +4936,11 @@
       </c>
       <c r="C29" s="94">
         <f t="shared" ref="C29:C54" ca="1" si="2">ROUND(MAX(MIN(100, NORMINV(RAND(), $H$8, $I$8)),0), 2)</f>
-        <v>77.78</v>
+        <v>80.55</v>
       </c>
       <c r="D29">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C31)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E29" s="33">
         <f>LN('Raw Data'!C31)</f>
@@ -4957,11 +4957,11 @@
       </c>
       <c r="C30" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>84.85</v>
+        <v>92.17</v>
       </c>
       <c r="D30">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C32)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E30" s="33">
         <f>LN('Raw Data'!C32)</f>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="C31" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>35.07</v>
+        <v>59.91</v>
       </c>
       <c r="D31">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C33)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
@@ -4999,11 +4999,11 @@
       </c>
       <c r="C32" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>59.71</v>
+        <v>65.92</v>
       </c>
       <c r="D32">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C34)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E32" s="33">
         <f>LN('Raw Data'!C34)</f>
@@ -5020,11 +5020,11 @@
       </c>
       <c r="C33" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>62.36</v>
+        <v>81.5</v>
       </c>
       <c r="D33">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C35)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E33" s="33">
         <f>LN('Raw Data'!C35)</f>
@@ -5041,11 +5041,11 @@
       </c>
       <c r="C34" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>81.83</v>
+        <v>57.76</v>
       </c>
       <c r="D34">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C36)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E34" s="33">
         <f>LN('Raw Data'!C36)</f>
@@ -5062,11 +5062,11 @@
       </c>
       <c r="C35" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>34.1</v>
+        <v>78.209999999999994</v>
       </c>
       <c r="D35">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C37)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E35" s="33">
         <f>LN('Raw Data'!C37)</f>
@@ -5083,11 +5083,11 @@
       </c>
       <c r="C36" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>50.63</v>
+        <v>26.18</v>
       </c>
       <c r="D36">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C38)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E36" s="33">
         <f>LN('Raw Data'!C38)</f>
@@ -5104,11 +5104,11 @@
       </c>
       <c r="C37" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>69.14</v>
+        <v>53.86</v>
       </c>
       <c r="D37">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C39)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E37" s="33">
         <f>LN('Raw Data'!C39)</f>
@@ -5125,11 +5125,11 @@
       </c>
       <c r="C38" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>58.15</v>
+        <v>74.48</v>
       </c>
       <c r="D38">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C40)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E38" s="33">
         <f>LN('Raw Data'!C40)</f>
@@ -5146,11 +5146,11 @@
       </c>
       <c r="C39" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>71.55</v>
+        <v>72.34</v>
       </c>
       <c r="D39">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C41)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E39" s="33">
         <f>LN('Raw Data'!C41)</f>
@@ -5167,11 +5167,11 @@
       </c>
       <c r="C40" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>84.18</v>
+        <v>53.36</v>
       </c>
       <c r="D40">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C42)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E40" s="33">
         <f>LN('Raw Data'!C42)</f>
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C41" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>46.78</v>
+        <v>69.989999999999995</v>
       </c>
       <c r="D41">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C43)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E41" s="33">
         <f>LN('Raw Data'!C43)</f>
@@ -5209,11 +5209,11 @@
       </c>
       <c r="C42" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>60.32</v>
+        <v>48.21</v>
       </c>
       <c r="D42">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C44)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E42" s="33">
         <f>LN('Raw Data'!C44)</f>
@@ -5230,11 +5230,11 @@
       </c>
       <c r="C43" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>85.17</v>
+        <v>60.03</v>
       </c>
       <c r="D43">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C45)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E43" s="33">
         <f>LN('Raw Data'!C45)</f>
@@ -5251,11 +5251,11 @@
       </c>
       <c r="C44" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>29.63</v>
+        <v>55.97</v>
       </c>
       <c r="D44">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C46)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" s="33">
         <f>LN('Raw Data'!C46)</f>
@@ -5272,11 +5272,11 @@
       </c>
       <c r="C45" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>67.290000000000006</v>
       </c>
       <c r="D45">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C47)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E45" s="33">
         <f>LN('Raw Data'!C47)</f>
@@ -5293,11 +5293,11 @@
       </c>
       <c r="C46" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>21.4</v>
+        <v>89.33</v>
       </c>
       <c r="D46">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C48)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E46" s="33">
         <f>LN('Raw Data'!C48)</f>
@@ -5314,11 +5314,11 @@
       </c>
       <c r="C47" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>55.92</v>
+        <v>88.73</v>
       </c>
       <c r="D47">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C49)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E47" s="33">
         <f>LN('Raw Data'!C49)</f>
@@ -5335,11 +5335,11 @@
       </c>
       <c r="C48" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>55.08</v>
+        <v>55.27</v>
       </c>
       <c r="D48">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C50)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E48" s="33">
         <f>LN('Raw Data'!C50)</f>
@@ -5356,11 +5356,11 @@
       </c>
       <c r="C49" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>90.65</v>
+        <v>76.81</v>
       </c>
       <c r="D49">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C51)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E49" s="33">
         <f>LN('Raw Data'!C51)</f>
@@ -5377,11 +5377,11 @@
       </c>
       <c r="C50" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>65.23</v>
+        <v>57.2</v>
       </c>
       <c r="D50">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C52)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E50" s="33">
         <f>LN('Raw Data'!C52)</f>
@@ -5398,11 +5398,11 @@
       </c>
       <c r="C51" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>51.97</v>
+        <v>94.7</v>
       </c>
       <c r="D51">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C53)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E51" s="33">
         <f>LN('Raw Data'!C53)</f>
@@ -5419,11 +5419,11 @@
       </c>
       <c r="C52" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>26.13</v>
+        <v>100</v>
       </c>
       <c r="D52">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C54)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E52" s="33">
         <f>LN('Raw Data'!C54)</f>
@@ -5440,11 +5440,11 @@
       </c>
       <c r="C53" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>80.739999999999995</v>
+        <v>92.74</v>
       </c>
       <c r="D53">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C55)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E53" s="33">
         <f>LN('Raw Data'!C55)</f>
@@ -5461,11 +5461,11 @@
       </c>
       <c r="C54" s="94">
         <f t="shared" ca="1" si="2"/>
-        <v>73.53</v>
+        <v>33.47</v>
       </c>
       <c r="D54">
         <f ca="1">MAX(0, ROUND($H$12  + (100-'Raw Data'!C56)*$H$13 + NORMINV(RAND(), $H$11, $I$11),0))</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E54" s="33">
         <f>LN('Raw Data'!C56)</f>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="B59" s="33">
         <f ca="1">AVERAGEA($C$3:$C$28)</f>
-        <v>54.061538461538461</v>
+        <v>57.380769230769232</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -5514,7 +5514,7 @@
       </c>
       <c r="B60" s="33">
         <f ca="1">AVERAGEA($C$29:$C$54)</f>
-        <v>61.996153846153859</v>
+        <v>68.691538461538457</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="B61" s="33">
         <f ca="1">STDEVA($C$3:$C$28)</f>
-        <v>26.963257324337906</v>
+        <v>22.487625739161867</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13">
@@ -5532,7 +5532,7 @@
       </c>
       <c r="B62" s="33">
         <f ca="1">STDEVA($C$29:$C$54)</f>
-        <v>21.119273676321917</v>
+        <v>18.762761778012866</v>
       </c>
     </row>
   </sheetData>
@@ -8045,7 +8045,7 @@
   </sheetPr>
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="191" zoomScaleNormal="268" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -9658,7 +9658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA86947-E241-514A-AD1F-5C5A7FFCD94F}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>